<commit_message>
finalize transition of eff-tax-rates and snacomapare
</commit_message>
<xml_diff>
--- a/input_data/admin_data/COL/_clean/total-pos-COL.xlsx
+++ b/input_data/admin_data/COL/_clean/total-pos-COL.xlsx
@@ -22,7 +22,838 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="831">
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
   <si>
     <t>poptot</t>
   </si>
@@ -1736,31 +2567,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>277</v>
+        <v>554</v>
       </c>
       <c r="B1" t="s">
-        <v>278</v>
+        <v>555</v>
       </c>
       <c r="C1" t="s">
-        <v>279</v>
+        <v>556</v>
       </c>
       <c r="D1" t="s">
-        <v>280</v>
+        <v>557</v>
       </c>
       <c r="E1" t="s">
-        <v>281</v>
+        <v>558</v>
       </c>
       <c r="F1" t="s">
-        <v>282</v>
+        <v>559</v>
       </c>
       <c r="G1" t="s">
-        <v>283</v>
+        <v>560</v>
       </c>
       <c r="H1" t="s">
-        <v>284</v>
+        <v>561</v>
       </c>
       <c r="I1" t="s">
-        <v>285</v>
+        <v>562</v>
       </c>
     </row>
     <row r="2">
@@ -1789,7 +2620,7 @@
         <v>2014</v>
       </c>
       <c r="I2" t="s">
-        <v>286</v>
+        <v>563</v>
       </c>
     </row>
     <row r="3">
@@ -1816,7 +2647,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>287</v>
+        <v>564</v>
       </c>
     </row>
     <row r="4">
@@ -1843,7 +2674,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>288</v>
+        <v>565</v>
       </c>
     </row>
     <row r="5">
@@ -1870,7 +2701,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>289</v>
+        <v>566</v>
       </c>
     </row>
     <row r="6">
@@ -1897,7 +2728,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>290</v>
+        <v>567</v>
       </c>
     </row>
     <row r="7">
@@ -1924,7 +2755,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>291</v>
+        <v>568</v>
       </c>
     </row>
     <row r="8">
@@ -1951,7 +2782,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>292</v>
+        <v>569</v>
       </c>
     </row>
     <row r="9">
@@ -1978,7 +2809,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>293</v>
+        <v>570</v>
       </c>
     </row>
     <row r="10">
@@ -2005,7 +2836,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>294</v>
+        <v>571</v>
       </c>
     </row>
     <row r="11">
@@ -2032,7 +2863,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>295</v>
+        <v>572</v>
       </c>
     </row>
     <row r="12">
@@ -2059,7 +2890,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>296</v>
+        <v>573</v>
       </c>
     </row>
     <row r="13">
@@ -2086,7 +2917,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>297</v>
+        <v>574</v>
       </c>
     </row>
     <row r="14">
@@ -2113,7 +2944,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>298</v>
+        <v>575</v>
       </c>
     </row>
     <row r="15">
@@ -2140,7 +2971,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>299</v>
+        <v>576</v>
       </c>
     </row>
     <row r="16">
@@ -2167,7 +2998,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>300</v>
+        <v>577</v>
       </c>
     </row>
     <row r="17">
@@ -2194,7 +3025,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>301</v>
+        <v>578</v>
       </c>
     </row>
     <row r="18">
@@ -2221,7 +3052,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>302</v>
+        <v>579</v>
       </c>
     </row>
     <row r="19">
@@ -2248,7 +3079,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>303</v>
+        <v>580</v>
       </c>
     </row>
     <row r="20">
@@ -2275,7 +3106,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>304</v>
+        <v>581</v>
       </c>
     </row>
     <row r="21">
@@ -2302,7 +3133,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" t="s">
-        <v>305</v>
+        <v>582</v>
       </c>
     </row>
   </sheetData>
@@ -2316,31 +3147,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>526</v>
+        <v>803</v>
       </c>
       <c r="B1" t="s">
-        <v>527</v>
+        <v>804</v>
       </c>
       <c r="C1" t="s">
-        <v>528</v>
+        <v>805</v>
       </c>
       <c r="D1" t="s">
-        <v>529</v>
+        <v>806</v>
       </c>
       <c r="E1" t="s">
-        <v>530</v>
+        <v>807</v>
       </c>
       <c r="F1" t="s">
-        <v>531</v>
+        <v>808</v>
       </c>
       <c r="G1" t="s">
-        <v>532</v>
+        <v>809</v>
       </c>
       <c r="H1" t="s">
-        <v>533</v>
+        <v>810</v>
       </c>
       <c r="I1" t="s">
-        <v>534</v>
+        <v>811</v>
       </c>
     </row>
     <row r="2">
@@ -2369,7 +3200,7 @@
         <v>2023</v>
       </c>
       <c r="I2" t="s">
-        <v>535</v>
+        <v>812</v>
       </c>
     </row>
     <row r="3">
@@ -2396,7 +3227,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>536</v>
+        <v>813</v>
       </c>
     </row>
     <row r="4">
@@ -2423,7 +3254,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>537</v>
+        <v>814</v>
       </c>
     </row>
     <row r="5">
@@ -2450,7 +3281,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>538</v>
+        <v>815</v>
       </c>
     </row>
     <row r="6">
@@ -2477,7 +3308,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>539</v>
+        <v>816</v>
       </c>
     </row>
     <row r="7">
@@ -2504,7 +3335,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>540</v>
+        <v>817</v>
       </c>
     </row>
     <row r="8">
@@ -2531,7 +3362,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>541</v>
+        <v>818</v>
       </c>
     </row>
     <row r="9">
@@ -2558,7 +3389,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>542</v>
+        <v>819</v>
       </c>
     </row>
     <row r="10">
@@ -2585,7 +3416,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>543</v>
+        <v>820</v>
       </c>
     </row>
     <row r="11">
@@ -2612,7 +3443,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>544</v>
+        <v>821</v>
       </c>
     </row>
     <row r="12">
@@ -2639,7 +3470,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>545</v>
+        <v>822</v>
       </c>
     </row>
     <row r="13">
@@ -2666,7 +3497,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>546</v>
+        <v>823</v>
       </c>
     </row>
     <row r="14">
@@ -2693,7 +3524,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>547</v>
+        <v>824</v>
       </c>
     </row>
     <row r="15">
@@ -2720,7 +3551,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>548</v>
+        <v>825</v>
       </c>
     </row>
     <row r="16">
@@ -2747,7 +3578,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>549</v>
+        <v>826</v>
       </c>
     </row>
     <row r="17">
@@ -2774,7 +3605,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>550</v>
+        <v>827</v>
       </c>
     </row>
     <row r="18">
@@ -2801,7 +3632,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>551</v>
+        <v>828</v>
       </c>
     </row>
     <row r="19">
@@ -2828,7 +3659,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>552</v>
+        <v>829</v>
       </c>
     </row>
     <row r="20">
@@ -2855,7 +3686,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>553</v>
+        <v>830</v>
       </c>
     </row>
   </sheetData>
@@ -2869,31 +3700,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>306</v>
+        <v>583</v>
       </c>
       <c r="B1" t="s">
-        <v>307</v>
+        <v>584</v>
       </c>
       <c r="C1" t="s">
-        <v>308</v>
+        <v>585</v>
       </c>
       <c r="D1" t="s">
-        <v>309</v>
+        <v>586</v>
       </c>
       <c r="E1" t="s">
-        <v>310</v>
+        <v>587</v>
       </c>
       <c r="F1" t="s">
-        <v>311</v>
+        <v>588</v>
       </c>
       <c r="G1" t="s">
-        <v>312</v>
+        <v>589</v>
       </c>
       <c r="H1" t="s">
-        <v>313</v>
+        <v>590</v>
       </c>
       <c r="I1" t="s">
-        <v>314</v>
+        <v>591</v>
       </c>
     </row>
     <row r="2">
@@ -2922,7 +3753,7 @@
         <v>2015</v>
       </c>
       <c r="I2" t="s">
-        <v>315</v>
+        <v>592</v>
       </c>
     </row>
     <row r="3">
@@ -2949,7 +3780,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>316</v>
+        <v>593</v>
       </c>
     </row>
     <row r="4">
@@ -2976,7 +3807,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>317</v>
+        <v>594</v>
       </c>
     </row>
     <row r="5">
@@ -3003,7 +3834,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>318</v>
+        <v>595</v>
       </c>
     </row>
     <row r="6">
@@ -3030,7 +3861,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>319</v>
+        <v>596</v>
       </c>
     </row>
     <row r="7">
@@ -3057,7 +3888,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>320</v>
+        <v>597</v>
       </c>
     </row>
     <row r="8">
@@ -3084,7 +3915,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>321</v>
+        <v>598</v>
       </c>
     </row>
     <row r="9">
@@ -3111,7 +3942,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>322</v>
+        <v>599</v>
       </c>
     </row>
     <row r="10">
@@ -3138,7 +3969,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>323</v>
+        <v>600</v>
       </c>
     </row>
     <row r="11">
@@ -3165,7 +3996,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>324</v>
+        <v>601</v>
       </c>
     </row>
     <row r="12">
@@ -3192,7 +4023,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>325</v>
+        <v>602</v>
       </c>
     </row>
     <row r="13">
@@ -3219,7 +4050,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>326</v>
+        <v>603</v>
       </c>
     </row>
     <row r="14">
@@ -3246,7 +4077,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>327</v>
+        <v>604</v>
       </c>
     </row>
     <row r="15">
@@ -3273,7 +4104,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>328</v>
+        <v>605</v>
       </c>
     </row>
     <row r="16">
@@ -3300,7 +4131,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>329</v>
+        <v>606</v>
       </c>
     </row>
     <row r="17">
@@ -3327,7 +4158,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>330</v>
+        <v>607</v>
       </c>
     </row>
     <row r="18">
@@ -3354,7 +4185,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>331</v>
+        <v>608</v>
       </c>
     </row>
     <row r="19">
@@ -3381,7 +4212,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>332</v>
+        <v>609</v>
       </c>
     </row>
     <row r="20">
@@ -3408,7 +4239,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>333</v>
+        <v>610</v>
       </c>
     </row>
     <row r="21">
@@ -3435,7 +4266,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" t="s">
-        <v>334</v>
+        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -3449,31 +4280,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>335</v>
+        <v>612</v>
       </c>
       <c r="B1" t="s">
-        <v>336</v>
+        <v>613</v>
       </c>
       <c r="C1" t="s">
-        <v>337</v>
+        <v>614</v>
       </c>
       <c r="D1" t="s">
-        <v>338</v>
+        <v>615</v>
       </c>
       <c r="E1" t="s">
-        <v>339</v>
+        <v>616</v>
       </c>
       <c r="F1" t="s">
-        <v>340</v>
+        <v>617</v>
       </c>
       <c r="G1" t="s">
-        <v>341</v>
+        <v>618</v>
       </c>
       <c r="H1" t="s">
-        <v>342</v>
+        <v>619</v>
       </c>
       <c r="I1" t="s">
-        <v>343</v>
+        <v>620</v>
       </c>
     </row>
     <row r="2">
@@ -3502,7 +4333,7 @@
         <v>2016</v>
       </c>
       <c r="I2" t="s">
-        <v>344</v>
+        <v>621</v>
       </c>
     </row>
     <row r="3">
@@ -3529,7 +4360,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>345</v>
+        <v>622</v>
       </c>
     </row>
     <row r="4">
@@ -3556,7 +4387,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>346</v>
+        <v>623</v>
       </c>
     </row>
     <row r="5">
@@ -3583,7 +4414,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>347</v>
+        <v>624</v>
       </c>
     </row>
     <row r="6">
@@ -3610,7 +4441,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>348</v>
+        <v>625</v>
       </c>
     </row>
     <row r="7">
@@ -3637,7 +4468,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>349</v>
+        <v>626</v>
       </c>
     </row>
     <row r="8">
@@ -3664,7 +4495,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>350</v>
+        <v>627</v>
       </c>
     </row>
     <row r="9">
@@ -3691,7 +4522,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>351</v>
+        <v>628</v>
       </c>
     </row>
     <row r="10">
@@ -3718,7 +4549,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>352</v>
+        <v>629</v>
       </c>
     </row>
     <row r="11">
@@ -3745,7 +4576,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>353</v>
+        <v>630</v>
       </c>
     </row>
     <row r="12">
@@ -3772,7 +4603,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>354</v>
+        <v>631</v>
       </c>
     </row>
     <row r="13">
@@ -3799,7 +4630,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>355</v>
+        <v>632</v>
       </c>
     </row>
     <row r="14">
@@ -3826,7 +4657,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>356</v>
+        <v>633</v>
       </c>
     </row>
     <row r="15">
@@ -3853,7 +4684,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>357</v>
+        <v>634</v>
       </c>
     </row>
     <row r="16">
@@ -3880,7 +4711,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>358</v>
+        <v>635</v>
       </c>
     </row>
     <row r="17">
@@ -3907,7 +4738,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>359</v>
+        <v>636</v>
       </c>
     </row>
     <row r="18">
@@ -3934,7 +4765,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>360</v>
+        <v>637</v>
       </c>
     </row>
     <row r="19">
@@ -3961,7 +4792,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>361</v>
+        <v>638</v>
       </c>
     </row>
     <row r="20">
@@ -3988,7 +4819,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>362</v>
+        <v>639</v>
       </c>
     </row>
     <row r="21">
@@ -4015,7 +4846,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" t="s">
-        <v>363</v>
+        <v>640</v>
       </c>
     </row>
     <row r="22">
@@ -4042,7 +4873,7 @@
       </c>
       <c r="H22" s="1"/>
       <c r="I22" t="s">
-        <v>364</v>
+        <v>641</v>
       </c>
     </row>
   </sheetData>
@@ -4056,31 +4887,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>365</v>
+        <v>642</v>
       </c>
       <c r="B1" t="s">
-        <v>366</v>
+        <v>643</v>
       </c>
       <c r="C1" t="s">
-        <v>367</v>
+        <v>644</v>
       </c>
       <c r="D1" t="s">
-        <v>368</v>
+        <v>645</v>
       </c>
       <c r="E1" t="s">
-        <v>369</v>
+        <v>646</v>
       </c>
       <c r="F1" t="s">
-        <v>370</v>
+        <v>647</v>
       </c>
       <c r="G1" t="s">
-        <v>371</v>
+        <v>648</v>
       </c>
       <c r="H1" t="s">
-        <v>372</v>
+        <v>649</v>
       </c>
       <c r="I1" t="s">
-        <v>373</v>
+        <v>650</v>
       </c>
     </row>
     <row r="2">
@@ -4109,7 +4940,7 @@
         <v>2017</v>
       </c>
       <c r="I2" t="s">
-        <v>374</v>
+        <v>651</v>
       </c>
     </row>
     <row r="3">
@@ -4136,7 +4967,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>375</v>
+        <v>652</v>
       </c>
     </row>
     <row r="4">
@@ -4163,7 +4994,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>376</v>
+        <v>653</v>
       </c>
     </row>
     <row r="5">
@@ -4190,7 +5021,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>377</v>
+        <v>654</v>
       </c>
     </row>
     <row r="6">
@@ -4217,7 +5048,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>378</v>
+        <v>655</v>
       </c>
     </row>
     <row r="7">
@@ -4244,7 +5075,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>379</v>
+        <v>656</v>
       </c>
     </row>
     <row r="8">
@@ -4271,7 +5102,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>380</v>
+        <v>657</v>
       </c>
     </row>
     <row r="9">
@@ -4298,7 +5129,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>381</v>
+        <v>658</v>
       </c>
     </row>
     <row r="10">
@@ -4325,7 +5156,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>382</v>
+        <v>659</v>
       </c>
     </row>
     <row r="11">
@@ -4352,7 +5183,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>383</v>
+        <v>660</v>
       </c>
     </row>
     <row r="12">
@@ -4379,7 +5210,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>384</v>
+        <v>661</v>
       </c>
     </row>
     <row r="13">
@@ -4406,7 +5237,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>385</v>
+        <v>662</v>
       </c>
     </row>
     <row r="14">
@@ -4433,7 +5264,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>386</v>
+        <v>663</v>
       </c>
     </row>
     <row r="15">
@@ -4460,7 +5291,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>387</v>
+        <v>664</v>
       </c>
     </row>
     <row r="16">
@@ -4487,7 +5318,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>388</v>
+        <v>665</v>
       </c>
     </row>
     <row r="17">
@@ -4514,7 +5345,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>389</v>
+        <v>666</v>
       </c>
     </row>
     <row r="18">
@@ -4541,7 +5372,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>390</v>
+        <v>667</v>
       </c>
     </row>
     <row r="19">
@@ -4568,7 +5399,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>391</v>
+        <v>668</v>
       </c>
     </row>
     <row r="20">
@@ -4595,7 +5426,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>392</v>
+        <v>669</v>
       </c>
     </row>
   </sheetData>
@@ -4609,31 +5440,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>393</v>
+        <v>670</v>
       </c>
       <c r="B1" t="s">
-        <v>394</v>
+        <v>671</v>
       </c>
       <c r="C1" t="s">
-        <v>395</v>
+        <v>672</v>
       </c>
       <c r="D1" t="s">
-        <v>396</v>
+        <v>673</v>
       </c>
       <c r="E1" t="s">
-        <v>397</v>
+        <v>674</v>
       </c>
       <c r="F1" t="s">
-        <v>398</v>
+        <v>675</v>
       </c>
       <c r="G1" t="s">
-        <v>399</v>
+        <v>676</v>
       </c>
       <c r="H1" t="s">
-        <v>400</v>
+        <v>677</v>
       </c>
       <c r="I1" t="s">
-        <v>401</v>
+        <v>678</v>
       </c>
     </row>
     <row r="2">
@@ -4662,7 +5493,7 @@
         <v>2018</v>
       </c>
       <c r="I2" t="s">
-        <v>402</v>
+        <v>679</v>
       </c>
     </row>
     <row r="3">
@@ -4689,7 +5520,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>403</v>
+        <v>680</v>
       </c>
     </row>
     <row r="4">
@@ -4716,7 +5547,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>404</v>
+        <v>681</v>
       </c>
     </row>
     <row r="5">
@@ -4743,7 +5574,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>405</v>
+        <v>682</v>
       </c>
     </row>
     <row r="6">
@@ -4770,7 +5601,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>406</v>
+        <v>683</v>
       </c>
     </row>
     <row r="7">
@@ -4797,7 +5628,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>407</v>
+        <v>684</v>
       </c>
     </row>
     <row r="8">
@@ -4824,7 +5655,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>408</v>
+        <v>685</v>
       </c>
     </row>
     <row r="9">
@@ -4851,7 +5682,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>409</v>
+        <v>686</v>
       </c>
     </row>
     <row r="10">
@@ -4878,7 +5709,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>410</v>
+        <v>687</v>
       </c>
     </row>
     <row r="11">
@@ -4905,7 +5736,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>411</v>
+        <v>688</v>
       </c>
     </row>
     <row r="12">
@@ -4932,7 +5763,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>412</v>
+        <v>689</v>
       </c>
     </row>
     <row r="13">
@@ -4959,7 +5790,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>413</v>
+        <v>690</v>
       </c>
     </row>
     <row r="14">
@@ -4986,7 +5817,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>414</v>
+        <v>691</v>
       </c>
     </row>
     <row r="15">
@@ -5013,7 +5844,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>415</v>
+        <v>692</v>
       </c>
     </row>
     <row r="16">
@@ -5040,7 +5871,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>416</v>
+        <v>693</v>
       </c>
     </row>
     <row r="17">
@@ -5067,7 +5898,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>417</v>
+        <v>694</v>
       </c>
     </row>
     <row r="18">
@@ -5094,7 +5925,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>418</v>
+        <v>695</v>
       </c>
     </row>
     <row r="19">
@@ -5121,7 +5952,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>419</v>
+        <v>696</v>
       </c>
     </row>
   </sheetData>
@@ -5135,31 +5966,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>420</v>
+        <v>697</v>
       </c>
       <c r="B1" t="s">
-        <v>421</v>
+        <v>698</v>
       </c>
       <c r="C1" t="s">
-        <v>422</v>
+        <v>699</v>
       </c>
       <c r="D1" t="s">
-        <v>423</v>
+        <v>700</v>
       </c>
       <c r="E1" t="s">
-        <v>424</v>
+        <v>701</v>
       </c>
       <c r="F1" t="s">
-        <v>425</v>
+        <v>702</v>
       </c>
       <c r="G1" t="s">
-        <v>426</v>
+        <v>703</v>
       </c>
       <c r="H1" t="s">
-        <v>427</v>
+        <v>704</v>
       </c>
       <c r="I1" t="s">
-        <v>428</v>
+        <v>705</v>
       </c>
     </row>
     <row r="2">
@@ -5188,7 +6019,7 @@
         <v>2019</v>
       </c>
       <c r="I2" t="s">
-        <v>429</v>
+        <v>706</v>
       </c>
     </row>
     <row r="3">
@@ -5215,7 +6046,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>430</v>
+        <v>707</v>
       </c>
     </row>
     <row r="4">
@@ -5242,7 +6073,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>431</v>
+        <v>708</v>
       </c>
     </row>
     <row r="5">
@@ -5269,7 +6100,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>432</v>
+        <v>709</v>
       </c>
     </row>
     <row r="6">
@@ -5296,7 +6127,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>433</v>
+        <v>710</v>
       </c>
     </row>
     <row r="7">
@@ -5323,7 +6154,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>434</v>
+        <v>711</v>
       </c>
     </row>
     <row r="8">
@@ -5350,7 +6181,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>435</v>
+        <v>712</v>
       </c>
     </row>
     <row r="9">
@@ -5377,7 +6208,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>436</v>
+        <v>713</v>
       </c>
     </row>
     <row r="10">
@@ -5404,7 +6235,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>437</v>
+        <v>714</v>
       </c>
     </row>
     <row r="11">
@@ -5431,7 +6262,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>438</v>
+        <v>715</v>
       </c>
     </row>
     <row r="12">
@@ -5458,7 +6289,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>439</v>
+        <v>716</v>
       </c>
     </row>
     <row r="13">
@@ -5485,7 +6316,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>440</v>
+        <v>717</v>
       </c>
     </row>
     <row r="14">
@@ -5512,7 +6343,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>441</v>
+        <v>718</v>
       </c>
     </row>
     <row r="15">
@@ -5539,7 +6370,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>442</v>
+        <v>719</v>
       </c>
     </row>
     <row r="16">
@@ -5566,7 +6397,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>443</v>
+        <v>720</v>
       </c>
     </row>
     <row r="17">
@@ -5593,7 +6424,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>444</v>
+        <v>721</v>
       </c>
     </row>
     <row r="18">
@@ -5620,7 +6451,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>445</v>
+        <v>722</v>
       </c>
     </row>
     <row r="19">
@@ -5647,7 +6478,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>446</v>
+        <v>723</v>
       </c>
     </row>
   </sheetData>
@@ -5661,31 +6492,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>447</v>
+        <v>724</v>
       </c>
       <c r="B1" t="s">
-        <v>448</v>
+        <v>725</v>
       </c>
       <c r="C1" t="s">
-        <v>449</v>
+        <v>726</v>
       </c>
       <c r="D1" t="s">
-        <v>450</v>
+        <v>727</v>
       </c>
       <c r="E1" t="s">
-        <v>451</v>
+        <v>728</v>
       </c>
       <c r="F1" t="s">
-        <v>452</v>
+        <v>729</v>
       </c>
       <c r="G1" t="s">
-        <v>453</v>
+        <v>730</v>
       </c>
       <c r="H1" t="s">
-        <v>454</v>
+        <v>731</v>
       </c>
       <c r="I1" t="s">
-        <v>455</v>
+        <v>732</v>
       </c>
     </row>
     <row r="2">
@@ -5714,7 +6545,7 @@
         <v>2020</v>
       </c>
       <c r="I2" t="s">
-        <v>456</v>
+        <v>733</v>
       </c>
     </row>
     <row r="3">
@@ -5741,7 +6572,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>457</v>
+        <v>734</v>
       </c>
     </row>
     <row r="4">
@@ -5768,7 +6599,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>458</v>
+        <v>735</v>
       </c>
     </row>
     <row r="5">
@@ -5795,7 +6626,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>459</v>
+        <v>736</v>
       </c>
     </row>
     <row r="6">
@@ -5822,7 +6653,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>460</v>
+        <v>737</v>
       </c>
     </row>
     <row r="7">
@@ -5849,7 +6680,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>461</v>
+        <v>738</v>
       </c>
     </row>
     <row r="8">
@@ -5876,7 +6707,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>462</v>
+        <v>739</v>
       </c>
     </row>
     <row r="9">
@@ -5903,7 +6734,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>463</v>
+        <v>740</v>
       </c>
     </row>
     <row r="10">
@@ -5930,7 +6761,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>464</v>
+        <v>741</v>
       </c>
     </row>
     <row r="11">
@@ -5957,7 +6788,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>465</v>
+        <v>742</v>
       </c>
     </row>
     <row r="12">
@@ -5984,7 +6815,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>466</v>
+        <v>743</v>
       </c>
     </row>
     <row r="13">
@@ -6011,7 +6842,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>467</v>
+        <v>744</v>
       </c>
     </row>
     <row r="14">
@@ -6038,7 +6869,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>468</v>
+        <v>745</v>
       </c>
     </row>
     <row r="15">
@@ -6065,7 +6896,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>469</v>
+        <v>746</v>
       </c>
     </row>
     <row r="16">
@@ -6092,7 +6923,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>470</v>
+        <v>747</v>
       </c>
     </row>
     <row r="17">
@@ -6119,7 +6950,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>471</v>
+        <v>748</v>
       </c>
     </row>
     <row r="18">
@@ -6146,7 +6977,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>472</v>
+        <v>749</v>
       </c>
     </row>
   </sheetData>
@@ -6160,31 +6991,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>473</v>
+        <v>750</v>
       </c>
       <c r="B1" t="s">
-        <v>474</v>
+        <v>751</v>
       </c>
       <c r="C1" t="s">
-        <v>475</v>
+        <v>752</v>
       </c>
       <c r="D1" t="s">
-        <v>476</v>
+        <v>753</v>
       </c>
       <c r="E1" t="s">
-        <v>477</v>
+        <v>754</v>
       </c>
       <c r="F1" t="s">
-        <v>478</v>
+        <v>755</v>
       </c>
       <c r="G1" t="s">
-        <v>479</v>
+        <v>756</v>
       </c>
       <c r="H1" t="s">
-        <v>480</v>
+        <v>757</v>
       </c>
       <c r="I1" t="s">
-        <v>481</v>
+        <v>758</v>
       </c>
     </row>
     <row r="2">
@@ -6213,7 +7044,7 @@
         <v>2021</v>
       </c>
       <c r="I2" t="s">
-        <v>482</v>
+        <v>759</v>
       </c>
     </row>
     <row r="3">
@@ -6240,7 +7071,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>483</v>
+        <v>760</v>
       </c>
     </row>
     <row r="4">
@@ -6267,7 +7098,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>484</v>
+        <v>761</v>
       </c>
     </row>
     <row r="5">
@@ -6294,7 +7125,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>485</v>
+        <v>762</v>
       </c>
     </row>
     <row r="6">
@@ -6321,7 +7152,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>486</v>
+        <v>763</v>
       </c>
     </row>
     <row r="7">
@@ -6348,7 +7179,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>487</v>
+        <v>764</v>
       </c>
     </row>
     <row r="8">
@@ -6375,7 +7206,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>488</v>
+        <v>765</v>
       </c>
     </row>
     <row r="9">
@@ -6402,7 +7233,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>489</v>
+        <v>766</v>
       </c>
     </row>
     <row r="10">
@@ -6429,7 +7260,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>490</v>
+        <v>767</v>
       </c>
     </row>
     <row r="11">
@@ -6456,7 +7287,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>491</v>
+        <v>768</v>
       </c>
     </row>
     <row r="12">
@@ -6483,7 +7314,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>492</v>
+        <v>769</v>
       </c>
     </row>
     <row r="13">
@@ -6510,7 +7341,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>493</v>
+        <v>770</v>
       </c>
     </row>
     <row r="14">
@@ -6537,7 +7368,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>494</v>
+        <v>771</v>
       </c>
     </row>
     <row r="15">
@@ -6564,7 +7395,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>495</v>
+        <v>772</v>
       </c>
     </row>
     <row r="16">
@@ -6591,7 +7422,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>496</v>
+        <v>773</v>
       </c>
     </row>
     <row r="17">
@@ -6618,7 +7449,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>497</v>
+        <v>774</v>
       </c>
     </row>
     <row r="18">
@@ -6645,7 +7476,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>498</v>
+        <v>775</v>
       </c>
     </row>
   </sheetData>
@@ -6659,31 +7490,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>499</v>
+        <v>776</v>
       </c>
       <c r="B1" t="s">
-        <v>500</v>
+        <v>777</v>
       </c>
       <c r="C1" t="s">
-        <v>501</v>
+        <v>778</v>
       </c>
       <c r="D1" t="s">
-        <v>502</v>
+        <v>779</v>
       </c>
       <c r="E1" t="s">
-        <v>503</v>
+        <v>780</v>
       </c>
       <c r="F1" t="s">
-        <v>504</v>
+        <v>781</v>
       </c>
       <c r="G1" t="s">
-        <v>505</v>
+        <v>782</v>
       </c>
       <c r="H1" t="s">
-        <v>506</v>
+        <v>783</v>
       </c>
       <c r="I1" t="s">
-        <v>507</v>
+        <v>784</v>
       </c>
     </row>
     <row r="2">
@@ -6712,7 +7543,7 @@
         <v>2022</v>
       </c>
       <c r="I2" t="s">
-        <v>508</v>
+        <v>785</v>
       </c>
     </row>
     <row r="3">
@@ -6739,7 +7570,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>509</v>
+        <v>786</v>
       </c>
     </row>
     <row r="4">
@@ -6766,7 +7597,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>510</v>
+        <v>787</v>
       </c>
     </row>
     <row r="5">
@@ -6793,7 +7624,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>511</v>
+        <v>788</v>
       </c>
     </row>
     <row r="6">
@@ -6820,7 +7651,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>512</v>
+        <v>789</v>
       </c>
     </row>
     <row r="7">
@@ -6847,7 +7678,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>513</v>
+        <v>790</v>
       </c>
     </row>
     <row r="8">
@@ -6874,7 +7705,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>514</v>
+        <v>791</v>
       </c>
     </row>
     <row r="9">
@@ -6901,7 +7732,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>515</v>
+        <v>792</v>
       </c>
     </row>
     <row r="10">
@@ -6928,7 +7759,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>516</v>
+        <v>793</v>
       </c>
     </row>
     <row r="11">
@@ -6955,7 +7786,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>517</v>
+        <v>794</v>
       </c>
     </row>
     <row r="12">
@@ -6982,7 +7813,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>518</v>
+        <v>795</v>
       </c>
     </row>
     <row r="13">
@@ -7009,7 +7840,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>519</v>
+        <v>796</v>
       </c>
     </row>
     <row r="14">
@@ -7036,7 +7867,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>520</v>
+        <v>797</v>
       </c>
     </row>
     <row r="15">
@@ -7063,7 +7894,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>521</v>
+        <v>798</v>
       </c>
     </row>
     <row r="16">
@@ -7090,7 +7921,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>522</v>
+        <v>799</v>
       </c>
     </row>
     <row r="17">
@@ -7117,7 +7948,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>523</v>
+        <v>800</v>
       </c>
     </row>
     <row r="18">
@@ -7144,7 +7975,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>524</v>
+        <v>801</v>
       </c>
     </row>
     <row r="19">
@@ -7171,7 +8002,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>525</v>
+        <v>802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish data export to WID
</commit_message>
<xml_diff>
--- a/input_data/admin_data/COL/_clean/total-pos-COL.xlsx
+++ b/input_data/admin_data/COL/_clean/total-pos-COL.xlsx
@@ -22,7 +22,838 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="1108">
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
   <si>
     <t>poptot</t>
   </si>
@@ -2567,31 +3398,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>554</v>
+        <v>831</v>
       </c>
       <c r="B1" t="s">
-        <v>555</v>
+        <v>832</v>
       </c>
       <c r="C1" t="s">
-        <v>556</v>
+        <v>833</v>
       </c>
       <c r="D1" t="s">
-        <v>557</v>
+        <v>834</v>
       </c>
       <c r="E1" t="s">
-        <v>558</v>
+        <v>835</v>
       </c>
       <c r="F1" t="s">
-        <v>559</v>
+        <v>836</v>
       </c>
       <c r="G1" t="s">
-        <v>560</v>
+        <v>837</v>
       </c>
       <c r="H1" t="s">
-        <v>561</v>
+        <v>838</v>
       </c>
       <c r="I1" t="s">
-        <v>562</v>
+        <v>839</v>
       </c>
     </row>
     <row r="2">
@@ -2620,7 +3451,7 @@
         <v>2014</v>
       </c>
       <c r="I2" t="s">
-        <v>563</v>
+        <v>840</v>
       </c>
     </row>
     <row r="3">
@@ -2647,7 +3478,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>564</v>
+        <v>841</v>
       </c>
     </row>
     <row r="4">
@@ -2674,7 +3505,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>565</v>
+        <v>842</v>
       </c>
     </row>
     <row r="5">
@@ -2701,7 +3532,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>566</v>
+        <v>843</v>
       </c>
     </row>
     <row r="6">
@@ -2728,7 +3559,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>567</v>
+        <v>844</v>
       </c>
     </row>
     <row r="7">
@@ -2755,7 +3586,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>568</v>
+        <v>845</v>
       </c>
     </row>
     <row r="8">
@@ -2782,7 +3613,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>569</v>
+        <v>846</v>
       </c>
     </row>
     <row r="9">
@@ -2809,7 +3640,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>570</v>
+        <v>847</v>
       </c>
     </row>
     <row r="10">
@@ -2836,7 +3667,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>571</v>
+        <v>848</v>
       </c>
     </row>
     <row r="11">
@@ -2863,7 +3694,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>572</v>
+        <v>849</v>
       </c>
     </row>
     <row r="12">
@@ -2890,7 +3721,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>573</v>
+        <v>850</v>
       </c>
     </row>
     <row r="13">
@@ -2917,7 +3748,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>574</v>
+        <v>851</v>
       </c>
     </row>
     <row r="14">
@@ -2944,7 +3775,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>575</v>
+        <v>852</v>
       </c>
     </row>
     <row r="15">
@@ -2971,7 +3802,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>576</v>
+        <v>853</v>
       </c>
     </row>
     <row r="16">
@@ -2998,7 +3829,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>577</v>
+        <v>854</v>
       </c>
     </row>
     <row r="17">
@@ -3025,7 +3856,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>578</v>
+        <v>855</v>
       </c>
     </row>
     <row r="18">
@@ -3052,7 +3883,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>579</v>
+        <v>856</v>
       </c>
     </row>
     <row r="19">
@@ -3079,7 +3910,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>580</v>
+        <v>857</v>
       </c>
     </row>
     <row r="20">
@@ -3106,7 +3937,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>581</v>
+        <v>858</v>
       </c>
     </row>
     <row r="21">
@@ -3133,7 +3964,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" t="s">
-        <v>582</v>
+        <v>859</v>
       </c>
     </row>
   </sheetData>
@@ -3147,31 +3978,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>803</v>
+        <v>1080</v>
       </c>
       <c r="B1" t="s">
-        <v>804</v>
+        <v>1081</v>
       </c>
       <c r="C1" t="s">
-        <v>805</v>
+        <v>1082</v>
       </c>
       <c r="D1" t="s">
-        <v>806</v>
+        <v>1083</v>
       </c>
       <c r="E1" t="s">
-        <v>807</v>
+        <v>1084</v>
       </c>
       <c r="F1" t="s">
-        <v>808</v>
+        <v>1085</v>
       </c>
       <c r="G1" t="s">
-        <v>809</v>
+        <v>1086</v>
       </c>
       <c r="H1" t="s">
-        <v>810</v>
+        <v>1087</v>
       </c>
       <c r="I1" t="s">
-        <v>811</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="2">
@@ -3200,7 +4031,7 @@
         <v>2023</v>
       </c>
       <c r="I2" t="s">
-        <v>812</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="3">
@@ -3227,7 +4058,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>813</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="4">
@@ -3254,7 +4085,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>814</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="5">
@@ -3281,7 +4112,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>815</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="6">
@@ -3308,7 +4139,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>816</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="7">
@@ -3335,7 +4166,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>817</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="8">
@@ -3362,7 +4193,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>818</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="9">
@@ -3389,7 +4220,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>819</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="10">
@@ -3416,7 +4247,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>820</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="11">
@@ -3443,7 +4274,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>821</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="12">
@@ -3470,7 +4301,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>822</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="13">
@@ -3497,7 +4328,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>823</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="14">
@@ -3524,7 +4355,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>824</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="15">
@@ -3551,7 +4382,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>825</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="16">
@@ -3578,7 +4409,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>826</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="17">
@@ -3605,7 +4436,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>827</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="18">
@@ -3632,7 +4463,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>828</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="19">
@@ -3659,7 +4490,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>829</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="20">
@@ -3686,7 +4517,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>830</v>
+        <v>1107</v>
       </c>
     </row>
   </sheetData>
@@ -3700,31 +4531,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>583</v>
+        <v>860</v>
       </c>
       <c r="B1" t="s">
-        <v>584</v>
+        <v>861</v>
       </c>
       <c r="C1" t="s">
-        <v>585</v>
+        <v>862</v>
       </c>
       <c r="D1" t="s">
-        <v>586</v>
+        <v>863</v>
       </c>
       <c r="E1" t="s">
-        <v>587</v>
+        <v>864</v>
       </c>
       <c r="F1" t="s">
-        <v>588</v>
+        <v>865</v>
       </c>
       <c r="G1" t="s">
-        <v>589</v>
+        <v>866</v>
       </c>
       <c r="H1" t="s">
-        <v>590</v>
+        <v>867</v>
       </c>
       <c r="I1" t="s">
-        <v>591</v>
+        <v>868</v>
       </c>
     </row>
     <row r="2">
@@ -3753,7 +4584,7 @@
         <v>2015</v>
       </c>
       <c r="I2" t="s">
-        <v>592</v>
+        <v>869</v>
       </c>
     </row>
     <row r="3">
@@ -3780,7 +4611,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>593</v>
+        <v>870</v>
       </c>
     </row>
     <row r="4">
@@ -3807,7 +4638,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>594</v>
+        <v>871</v>
       </c>
     </row>
     <row r="5">
@@ -3834,7 +4665,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>595</v>
+        <v>872</v>
       </c>
     </row>
     <row r="6">
@@ -3861,7 +4692,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>596</v>
+        <v>873</v>
       </c>
     </row>
     <row r="7">
@@ -3888,7 +4719,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>597</v>
+        <v>874</v>
       </c>
     </row>
     <row r="8">
@@ -3915,7 +4746,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>598</v>
+        <v>875</v>
       </c>
     </row>
     <row r="9">
@@ -3942,7 +4773,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>599</v>
+        <v>876</v>
       </c>
     </row>
     <row r="10">
@@ -3969,7 +4800,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>600</v>
+        <v>877</v>
       </c>
     </row>
     <row r="11">
@@ -3996,7 +4827,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>601</v>
+        <v>878</v>
       </c>
     </row>
     <row r="12">
@@ -4023,7 +4854,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>602</v>
+        <v>879</v>
       </c>
     </row>
     <row r="13">
@@ -4050,7 +4881,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>603</v>
+        <v>880</v>
       </c>
     </row>
     <row r="14">
@@ -4077,7 +4908,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>604</v>
+        <v>881</v>
       </c>
     </row>
     <row r="15">
@@ -4104,7 +4935,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>605</v>
+        <v>882</v>
       </c>
     </row>
     <row r="16">
@@ -4131,7 +4962,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>606</v>
+        <v>883</v>
       </c>
     </row>
     <row r="17">
@@ -4158,7 +4989,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>607</v>
+        <v>884</v>
       </c>
     </row>
     <row r="18">
@@ -4185,7 +5016,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>608</v>
+        <v>885</v>
       </c>
     </row>
     <row r="19">
@@ -4212,7 +5043,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>609</v>
+        <v>886</v>
       </c>
     </row>
     <row r="20">
@@ -4239,7 +5070,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>610</v>
+        <v>887</v>
       </c>
     </row>
     <row r="21">
@@ -4266,7 +5097,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" t="s">
-        <v>611</v>
+        <v>888</v>
       </c>
     </row>
   </sheetData>
@@ -4280,31 +5111,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>612</v>
+        <v>889</v>
       </c>
       <c r="B1" t="s">
-        <v>613</v>
+        <v>890</v>
       </c>
       <c r="C1" t="s">
-        <v>614</v>
+        <v>891</v>
       </c>
       <c r="D1" t="s">
-        <v>615</v>
+        <v>892</v>
       </c>
       <c r="E1" t="s">
-        <v>616</v>
+        <v>893</v>
       </c>
       <c r="F1" t="s">
-        <v>617</v>
+        <v>894</v>
       </c>
       <c r="G1" t="s">
-        <v>618</v>
+        <v>895</v>
       </c>
       <c r="H1" t="s">
-        <v>619</v>
+        <v>896</v>
       </c>
       <c r="I1" t="s">
-        <v>620</v>
+        <v>897</v>
       </c>
     </row>
     <row r="2">
@@ -4333,7 +5164,7 @@
         <v>2016</v>
       </c>
       <c r="I2" t="s">
-        <v>621</v>
+        <v>898</v>
       </c>
     </row>
     <row r="3">
@@ -4360,7 +5191,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>622</v>
+        <v>899</v>
       </c>
     </row>
     <row r="4">
@@ -4387,7 +5218,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>623</v>
+        <v>900</v>
       </c>
     </row>
     <row r="5">
@@ -4414,7 +5245,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>624</v>
+        <v>901</v>
       </c>
     </row>
     <row r="6">
@@ -4441,7 +5272,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>625</v>
+        <v>902</v>
       </c>
     </row>
     <row r="7">
@@ -4468,7 +5299,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>626</v>
+        <v>903</v>
       </c>
     </row>
     <row r="8">
@@ -4495,7 +5326,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>627</v>
+        <v>904</v>
       </c>
     </row>
     <row r="9">
@@ -4522,7 +5353,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>628</v>
+        <v>905</v>
       </c>
     </row>
     <row r="10">
@@ -4549,7 +5380,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>629</v>
+        <v>906</v>
       </c>
     </row>
     <row r="11">
@@ -4576,7 +5407,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>630</v>
+        <v>907</v>
       </c>
     </row>
     <row r="12">
@@ -4603,7 +5434,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>631</v>
+        <v>908</v>
       </c>
     </row>
     <row r="13">
@@ -4630,7 +5461,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>632</v>
+        <v>909</v>
       </c>
     </row>
     <row r="14">
@@ -4657,7 +5488,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>633</v>
+        <v>910</v>
       </c>
     </row>
     <row r="15">
@@ -4684,7 +5515,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>634</v>
+        <v>911</v>
       </c>
     </row>
     <row r="16">
@@ -4711,7 +5542,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>635</v>
+        <v>912</v>
       </c>
     </row>
     <row r="17">
@@ -4738,7 +5569,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>636</v>
+        <v>913</v>
       </c>
     </row>
     <row r="18">
@@ -4765,7 +5596,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>637</v>
+        <v>914</v>
       </c>
     </row>
     <row r="19">
@@ -4792,7 +5623,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>638</v>
+        <v>915</v>
       </c>
     </row>
     <row r="20">
@@ -4819,7 +5650,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>639</v>
+        <v>916</v>
       </c>
     </row>
     <row r="21">
@@ -4846,7 +5677,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" t="s">
-        <v>640</v>
+        <v>917</v>
       </c>
     </row>
     <row r="22">
@@ -4873,7 +5704,7 @@
       </c>
       <c r="H22" s="1"/>
       <c r="I22" t="s">
-        <v>641</v>
+        <v>918</v>
       </c>
     </row>
   </sheetData>
@@ -4887,31 +5718,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>642</v>
+        <v>919</v>
       </c>
       <c r="B1" t="s">
-        <v>643</v>
+        <v>920</v>
       </c>
       <c r="C1" t="s">
-        <v>644</v>
+        <v>921</v>
       </c>
       <c r="D1" t="s">
-        <v>645</v>
+        <v>922</v>
       </c>
       <c r="E1" t="s">
-        <v>646</v>
+        <v>923</v>
       </c>
       <c r="F1" t="s">
-        <v>647</v>
+        <v>924</v>
       </c>
       <c r="G1" t="s">
-        <v>648</v>
+        <v>925</v>
       </c>
       <c r="H1" t="s">
-        <v>649</v>
+        <v>926</v>
       </c>
       <c r="I1" t="s">
-        <v>650</v>
+        <v>927</v>
       </c>
     </row>
     <row r="2">
@@ -4940,7 +5771,7 @@
         <v>2017</v>
       </c>
       <c r="I2" t="s">
-        <v>651</v>
+        <v>928</v>
       </c>
     </row>
     <row r="3">
@@ -4967,7 +5798,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>652</v>
+        <v>929</v>
       </c>
     </row>
     <row r="4">
@@ -4994,7 +5825,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>653</v>
+        <v>930</v>
       </c>
     </row>
     <row r="5">
@@ -5021,7 +5852,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>654</v>
+        <v>931</v>
       </c>
     </row>
     <row r="6">
@@ -5048,7 +5879,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>655</v>
+        <v>932</v>
       </c>
     </row>
     <row r="7">
@@ -5075,7 +5906,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>656</v>
+        <v>933</v>
       </c>
     </row>
     <row r="8">
@@ -5102,7 +5933,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>657</v>
+        <v>934</v>
       </c>
     </row>
     <row r="9">
@@ -5129,7 +5960,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>658</v>
+        <v>935</v>
       </c>
     </row>
     <row r="10">
@@ -5156,7 +5987,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>659</v>
+        <v>936</v>
       </c>
     </row>
     <row r="11">
@@ -5183,7 +6014,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>660</v>
+        <v>937</v>
       </c>
     </row>
     <row r="12">
@@ -5210,7 +6041,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>661</v>
+        <v>938</v>
       </c>
     </row>
     <row r="13">
@@ -5237,7 +6068,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>662</v>
+        <v>939</v>
       </c>
     </row>
     <row r="14">
@@ -5264,7 +6095,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>663</v>
+        <v>940</v>
       </c>
     </row>
     <row r="15">
@@ -5291,7 +6122,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>664</v>
+        <v>941</v>
       </c>
     </row>
     <row r="16">
@@ -5318,7 +6149,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>665</v>
+        <v>942</v>
       </c>
     </row>
     <row r="17">
@@ -5345,7 +6176,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>666</v>
+        <v>943</v>
       </c>
     </row>
     <row r="18">
@@ -5372,7 +6203,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>667</v>
+        <v>944</v>
       </c>
     </row>
     <row r="19">
@@ -5399,7 +6230,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>668</v>
+        <v>945</v>
       </c>
     </row>
     <row r="20">
@@ -5426,7 +6257,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>669</v>
+        <v>946</v>
       </c>
     </row>
   </sheetData>
@@ -5440,31 +6271,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>670</v>
+        <v>947</v>
       </c>
       <c r="B1" t="s">
-        <v>671</v>
+        <v>948</v>
       </c>
       <c r="C1" t="s">
-        <v>672</v>
+        <v>949</v>
       </c>
       <c r="D1" t="s">
-        <v>673</v>
+        <v>950</v>
       </c>
       <c r="E1" t="s">
-        <v>674</v>
+        <v>951</v>
       </c>
       <c r="F1" t="s">
-        <v>675</v>
+        <v>952</v>
       </c>
       <c r="G1" t="s">
-        <v>676</v>
+        <v>953</v>
       </c>
       <c r="H1" t="s">
-        <v>677</v>
+        <v>954</v>
       </c>
       <c r="I1" t="s">
-        <v>678</v>
+        <v>955</v>
       </c>
     </row>
     <row r="2">
@@ -5493,7 +6324,7 @@
         <v>2018</v>
       </c>
       <c r="I2" t="s">
-        <v>679</v>
+        <v>956</v>
       </c>
     </row>
     <row r="3">
@@ -5520,7 +6351,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>680</v>
+        <v>957</v>
       </c>
     </row>
     <row r="4">
@@ -5547,7 +6378,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>681</v>
+        <v>958</v>
       </c>
     </row>
     <row r="5">
@@ -5574,7 +6405,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>682</v>
+        <v>959</v>
       </c>
     </row>
     <row r="6">
@@ -5601,7 +6432,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>683</v>
+        <v>960</v>
       </c>
     </row>
     <row r="7">
@@ -5628,7 +6459,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>684</v>
+        <v>961</v>
       </c>
     </row>
     <row r="8">
@@ -5655,7 +6486,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>685</v>
+        <v>962</v>
       </c>
     </row>
     <row r="9">
@@ -5682,7 +6513,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>686</v>
+        <v>963</v>
       </c>
     </row>
     <row r="10">
@@ -5709,7 +6540,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>687</v>
+        <v>964</v>
       </c>
     </row>
     <row r="11">
@@ -5736,7 +6567,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>688</v>
+        <v>965</v>
       </c>
     </row>
     <row r="12">
@@ -5763,7 +6594,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>689</v>
+        <v>966</v>
       </c>
     </row>
     <row r="13">
@@ -5790,7 +6621,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>690</v>
+        <v>967</v>
       </c>
     </row>
     <row r="14">
@@ -5817,7 +6648,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>691</v>
+        <v>968</v>
       </c>
     </row>
     <row r="15">
@@ -5844,7 +6675,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>692</v>
+        <v>969</v>
       </c>
     </row>
     <row r="16">
@@ -5871,7 +6702,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>693</v>
+        <v>970</v>
       </c>
     </row>
     <row r="17">
@@ -5898,7 +6729,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>694</v>
+        <v>971</v>
       </c>
     </row>
     <row r="18">
@@ -5925,7 +6756,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>695</v>
+        <v>972</v>
       </c>
     </row>
     <row r="19">
@@ -5952,7 +6783,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>696</v>
+        <v>973</v>
       </c>
     </row>
   </sheetData>
@@ -5966,31 +6797,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>697</v>
+        <v>974</v>
       </c>
       <c r="B1" t="s">
-        <v>698</v>
+        <v>975</v>
       </c>
       <c r="C1" t="s">
-        <v>699</v>
+        <v>976</v>
       </c>
       <c r="D1" t="s">
-        <v>700</v>
+        <v>977</v>
       </c>
       <c r="E1" t="s">
-        <v>701</v>
+        <v>978</v>
       </c>
       <c r="F1" t="s">
-        <v>702</v>
+        <v>979</v>
       </c>
       <c r="G1" t="s">
-        <v>703</v>
+        <v>980</v>
       </c>
       <c r="H1" t="s">
-        <v>704</v>
+        <v>981</v>
       </c>
       <c r="I1" t="s">
-        <v>705</v>
+        <v>982</v>
       </c>
     </row>
     <row r="2">
@@ -6019,7 +6850,7 @@
         <v>2019</v>
       </c>
       <c r="I2" t="s">
-        <v>706</v>
+        <v>983</v>
       </c>
     </row>
     <row r="3">
@@ -6046,7 +6877,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>707</v>
+        <v>984</v>
       </c>
     </row>
     <row r="4">
@@ -6073,7 +6904,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>708</v>
+        <v>985</v>
       </c>
     </row>
     <row r="5">
@@ -6100,7 +6931,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>709</v>
+        <v>986</v>
       </c>
     </row>
     <row r="6">
@@ -6127,7 +6958,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>710</v>
+        <v>987</v>
       </c>
     </row>
     <row r="7">
@@ -6154,7 +6985,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>711</v>
+        <v>988</v>
       </c>
     </row>
     <row r="8">
@@ -6181,7 +7012,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>712</v>
+        <v>989</v>
       </c>
     </row>
     <row r="9">
@@ -6208,7 +7039,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>713</v>
+        <v>990</v>
       </c>
     </row>
     <row r="10">
@@ -6235,7 +7066,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>714</v>
+        <v>991</v>
       </c>
     </row>
     <row r="11">
@@ -6262,7 +7093,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>715</v>
+        <v>992</v>
       </c>
     </row>
     <row r="12">
@@ -6289,7 +7120,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>716</v>
+        <v>993</v>
       </c>
     </row>
     <row r="13">
@@ -6316,7 +7147,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>717</v>
+        <v>994</v>
       </c>
     </row>
     <row r="14">
@@ -6343,7 +7174,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>718</v>
+        <v>995</v>
       </c>
     </row>
     <row r="15">
@@ -6370,7 +7201,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>719</v>
+        <v>996</v>
       </c>
     </row>
     <row r="16">
@@ -6397,7 +7228,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>720</v>
+        <v>997</v>
       </c>
     </row>
     <row r="17">
@@ -6424,7 +7255,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>721</v>
+        <v>998</v>
       </c>
     </row>
     <row r="18">
@@ -6451,7 +7282,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>722</v>
+        <v>999</v>
       </c>
     </row>
     <row r="19">
@@ -6478,7 +7309,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>723</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -6492,31 +7323,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>724</v>
+        <v>1001</v>
       </c>
       <c r="B1" t="s">
-        <v>725</v>
+        <v>1002</v>
       </c>
       <c r="C1" t="s">
-        <v>726</v>
+        <v>1003</v>
       </c>
       <c r="D1" t="s">
-        <v>727</v>
+        <v>1004</v>
       </c>
       <c r="E1" t="s">
-        <v>728</v>
+        <v>1005</v>
       </c>
       <c r="F1" t="s">
-        <v>729</v>
+        <v>1006</v>
       </c>
       <c r="G1" t="s">
-        <v>730</v>
+        <v>1007</v>
       </c>
       <c r="H1" t="s">
-        <v>731</v>
+        <v>1008</v>
       </c>
       <c r="I1" t="s">
-        <v>732</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="2">
@@ -6545,7 +7376,7 @@
         <v>2020</v>
       </c>
       <c r="I2" t="s">
-        <v>733</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="3">
@@ -6572,7 +7403,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>734</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="4">
@@ -6599,7 +7430,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>735</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="5">
@@ -6626,7 +7457,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>736</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="6">
@@ -6653,7 +7484,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>737</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="7">
@@ -6680,7 +7511,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>738</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="8">
@@ -6707,7 +7538,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>739</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="9">
@@ -6734,7 +7565,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>740</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="10">
@@ -6761,7 +7592,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>741</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="11">
@@ -6788,7 +7619,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>742</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="12">
@@ -6815,7 +7646,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>743</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="13">
@@ -6842,7 +7673,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>744</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="14">
@@ -6869,7 +7700,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>745</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="15">
@@ -6896,7 +7727,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>746</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="16">
@@ -6923,7 +7754,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>747</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="17">
@@ -6950,7 +7781,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>748</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="18">
@@ -6977,7 +7808,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>749</v>
+        <v>1026</v>
       </c>
     </row>
   </sheetData>
@@ -6991,31 +7822,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>750</v>
+        <v>1027</v>
       </c>
       <c r="B1" t="s">
-        <v>751</v>
+        <v>1028</v>
       </c>
       <c r="C1" t="s">
-        <v>752</v>
+        <v>1029</v>
       </c>
       <c r="D1" t="s">
-        <v>753</v>
+        <v>1030</v>
       </c>
       <c r="E1" t="s">
-        <v>754</v>
+        <v>1031</v>
       </c>
       <c r="F1" t="s">
-        <v>755</v>
+        <v>1032</v>
       </c>
       <c r="G1" t="s">
-        <v>756</v>
+        <v>1033</v>
       </c>
       <c r="H1" t="s">
-        <v>757</v>
+        <v>1034</v>
       </c>
       <c r="I1" t="s">
-        <v>758</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="2">
@@ -7044,7 +7875,7 @@
         <v>2021</v>
       </c>
       <c r="I2" t="s">
-        <v>759</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="3">
@@ -7071,7 +7902,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>760</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="4">
@@ -7098,7 +7929,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>761</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="5">
@@ -7125,7 +7956,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>762</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="6">
@@ -7152,7 +7983,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>763</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="7">
@@ -7179,7 +8010,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>764</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="8">
@@ -7206,7 +8037,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>765</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="9">
@@ -7233,7 +8064,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>766</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="10">
@@ -7260,7 +8091,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>767</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="11">
@@ -7287,7 +8118,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>768</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="12">
@@ -7314,7 +8145,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>769</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="13">
@@ -7341,7 +8172,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>770</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="14">
@@ -7368,7 +8199,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>771</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="15">
@@ -7395,7 +8226,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>772</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="16">
@@ -7422,7 +8253,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>773</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="17">
@@ -7449,7 +8280,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>774</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="18">
@@ -7476,7 +8307,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>775</v>
+        <v>1052</v>
       </c>
     </row>
   </sheetData>
@@ -7490,31 +8321,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>776</v>
+        <v>1053</v>
       </c>
       <c r="B1" t="s">
-        <v>777</v>
+        <v>1054</v>
       </c>
       <c r="C1" t="s">
-        <v>778</v>
+        <v>1055</v>
       </c>
       <c r="D1" t="s">
-        <v>779</v>
+        <v>1056</v>
       </c>
       <c r="E1" t="s">
-        <v>780</v>
+        <v>1057</v>
       </c>
       <c r="F1" t="s">
-        <v>781</v>
+        <v>1058</v>
       </c>
       <c r="G1" t="s">
-        <v>782</v>
+        <v>1059</v>
       </c>
       <c r="H1" t="s">
-        <v>783</v>
+        <v>1060</v>
       </c>
       <c r="I1" t="s">
-        <v>784</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="2">
@@ -7543,7 +8374,7 @@
         <v>2022</v>
       </c>
       <c r="I2" t="s">
-        <v>785</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="3">
@@ -7570,7 +8401,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>786</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="4">
@@ -7597,7 +8428,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>787</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="5">
@@ -7624,7 +8455,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>788</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="6">
@@ -7651,7 +8482,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>789</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="7">
@@ -7678,7 +8509,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>790</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="8">
@@ -7705,7 +8536,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>791</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="9">
@@ -7732,7 +8563,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>792</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="10">
@@ -7759,7 +8590,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>793</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="11">
@@ -7786,7 +8617,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>794</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="12">
@@ -7813,7 +8644,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>795</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="13">
@@ -7840,7 +8671,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>796</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="14">
@@ -7867,7 +8698,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>797</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="15">
@@ -7894,7 +8725,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>798</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="16">
@@ -7921,7 +8752,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>799</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="17">
@@ -7948,7 +8779,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>800</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="18">
@@ -7975,7 +8806,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>801</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="19">
@@ -8002,7 +8833,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>802</v>
+        <v>1079</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add gpinter correction and solve other bugs
Also solve CRI being ignored
Add yearly data quality  report
Include many treated admin data files
</commit_message>
<xml_diff>
--- a/input_data/admin_data/COL/_clean/total-pos-COL.xlsx
+++ b/input_data/admin_data/COL/_clean/total-pos-COL.xlsx
@@ -22,7 +22,2500 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3047" uniqueCount="3047">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3878" uniqueCount="3878">
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
   <si>
     <t>poptot</t>
   </si>
@@ -9215,31 +11708,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>2770</v>
+        <v>3601</v>
       </c>
       <c r="B1" t="s">
-        <v>2771</v>
+        <v>3602</v>
       </c>
       <c r="C1" t="s">
-        <v>2772</v>
+        <v>3603</v>
       </c>
       <c r="D1" t="s">
-        <v>2773</v>
+        <v>3604</v>
       </c>
       <c r="E1" t="s">
-        <v>2774</v>
+        <v>3605</v>
       </c>
       <c r="F1" t="s">
-        <v>2775</v>
+        <v>3606</v>
       </c>
       <c r="G1" t="s">
-        <v>2776</v>
+        <v>3607</v>
       </c>
       <c r="H1" t="s">
-        <v>2777</v>
+        <v>3608</v>
       </c>
       <c r="I1" t="s">
-        <v>2778</v>
+        <v>3609</v>
       </c>
     </row>
     <row r="2">
@@ -9268,7 +11761,7 @@
         <v>2014</v>
       </c>
       <c r="I2" t="s">
-        <v>2779</v>
+        <v>3610</v>
       </c>
     </row>
     <row r="3">
@@ -9295,7 +11788,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>2780</v>
+        <v>3611</v>
       </c>
     </row>
     <row r="4">
@@ -9322,7 +11815,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>2781</v>
+        <v>3612</v>
       </c>
     </row>
     <row r="5">
@@ -9349,7 +11842,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>2782</v>
+        <v>3613</v>
       </c>
     </row>
     <row r="6">
@@ -9376,7 +11869,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>2783</v>
+        <v>3614</v>
       </c>
     </row>
     <row r="7">
@@ -9403,7 +11896,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>2784</v>
+        <v>3615</v>
       </c>
     </row>
     <row r="8">
@@ -9430,7 +11923,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>2785</v>
+        <v>3616</v>
       </c>
     </row>
     <row r="9">
@@ -9457,7 +11950,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>2786</v>
+        <v>3617</v>
       </c>
     </row>
     <row r="10">
@@ -9484,7 +11977,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>2787</v>
+        <v>3618</v>
       </c>
     </row>
     <row r="11">
@@ -9511,7 +12004,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>2788</v>
+        <v>3619</v>
       </c>
     </row>
     <row r="12">
@@ -9538,7 +12031,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>2789</v>
+        <v>3620</v>
       </c>
     </row>
     <row r="13">
@@ -9565,7 +12058,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>2790</v>
+        <v>3621</v>
       </c>
     </row>
     <row r="14">
@@ -9592,7 +12085,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>2791</v>
+        <v>3622</v>
       </c>
     </row>
     <row r="15">
@@ -9619,7 +12112,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>2792</v>
+        <v>3623</v>
       </c>
     </row>
     <row r="16">
@@ -9646,7 +12139,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>2793</v>
+        <v>3624</v>
       </c>
     </row>
     <row r="17">
@@ -9673,7 +12166,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>2794</v>
+        <v>3625</v>
       </c>
     </row>
     <row r="18">
@@ -9700,7 +12193,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>2795</v>
+        <v>3626</v>
       </c>
     </row>
     <row r="19">
@@ -9727,7 +12220,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>2796</v>
+        <v>3627</v>
       </c>
     </row>
     <row r="20">
@@ -9754,7 +12247,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>2797</v>
+        <v>3628</v>
       </c>
     </row>
     <row r="21">
@@ -9781,7 +12274,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" t="s">
-        <v>2798</v>
+        <v>3629</v>
       </c>
     </row>
   </sheetData>
@@ -9795,31 +12288,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>3019</v>
+        <v>3850</v>
       </c>
       <c r="B1" t="s">
-        <v>3020</v>
+        <v>3851</v>
       </c>
       <c r="C1" t="s">
-        <v>3021</v>
+        <v>3852</v>
       </c>
       <c r="D1" t="s">
-        <v>3022</v>
+        <v>3853</v>
       </c>
       <c r="E1" t="s">
-        <v>3023</v>
+        <v>3854</v>
       </c>
       <c r="F1" t="s">
-        <v>3024</v>
+        <v>3855</v>
       </c>
       <c r="G1" t="s">
-        <v>3025</v>
+        <v>3856</v>
       </c>
       <c r="H1" t="s">
-        <v>3026</v>
+        <v>3857</v>
       </c>
       <c r="I1" t="s">
-        <v>3027</v>
+        <v>3858</v>
       </c>
     </row>
     <row r="2">
@@ -9848,7 +12341,7 @@
         <v>2023</v>
       </c>
       <c r="I2" t="s">
-        <v>3028</v>
+        <v>3859</v>
       </c>
     </row>
     <row r="3">
@@ -9875,7 +12368,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>3029</v>
+        <v>3860</v>
       </c>
     </row>
     <row r="4">
@@ -9902,7 +12395,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>3030</v>
+        <v>3861</v>
       </c>
     </row>
     <row r="5">
@@ -9929,7 +12422,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>3031</v>
+        <v>3862</v>
       </c>
     </row>
     <row r="6">
@@ -9956,7 +12449,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>3032</v>
+        <v>3863</v>
       </c>
     </row>
     <row r="7">
@@ -9983,7 +12476,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>3033</v>
+        <v>3864</v>
       </c>
     </row>
     <row r="8">
@@ -10010,7 +12503,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>3034</v>
+        <v>3865</v>
       </c>
     </row>
     <row r="9">
@@ -10037,7 +12530,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>3035</v>
+        <v>3866</v>
       </c>
     </row>
     <row r="10">
@@ -10064,7 +12557,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>3036</v>
+        <v>3867</v>
       </c>
     </row>
     <row r="11">
@@ -10091,7 +12584,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>3037</v>
+        <v>3868</v>
       </c>
     </row>
     <row r="12">
@@ -10118,7 +12611,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>3038</v>
+        <v>3869</v>
       </c>
     </row>
     <row r="13">
@@ -10145,7 +12638,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>3039</v>
+        <v>3870</v>
       </c>
     </row>
     <row r="14">
@@ -10172,7 +12665,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>3040</v>
+        <v>3871</v>
       </c>
     </row>
     <row r="15">
@@ -10199,7 +12692,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>3041</v>
+        <v>3872</v>
       </c>
     </row>
     <row r="16">
@@ -10226,7 +12719,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>3042</v>
+        <v>3873</v>
       </c>
     </row>
     <row r="17">
@@ -10253,7 +12746,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>3043</v>
+        <v>3874</v>
       </c>
     </row>
     <row r="18">
@@ -10280,7 +12773,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>3044</v>
+        <v>3875</v>
       </c>
     </row>
     <row r="19">
@@ -10307,7 +12800,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>3045</v>
+        <v>3876</v>
       </c>
     </row>
     <row r="20">
@@ -10334,7 +12827,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>3046</v>
+        <v>3877</v>
       </c>
     </row>
   </sheetData>
@@ -10348,31 +12841,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>2799</v>
+        <v>3630</v>
       </c>
       <c r="B1" t="s">
-        <v>2800</v>
+        <v>3631</v>
       </c>
       <c r="C1" t="s">
-        <v>2801</v>
+        <v>3632</v>
       </c>
       <c r="D1" t="s">
-        <v>2802</v>
+        <v>3633</v>
       </c>
       <c r="E1" t="s">
-        <v>2803</v>
+        <v>3634</v>
       </c>
       <c r="F1" t="s">
-        <v>2804</v>
+        <v>3635</v>
       </c>
       <c r="G1" t="s">
-        <v>2805</v>
+        <v>3636</v>
       </c>
       <c r="H1" t="s">
-        <v>2806</v>
+        <v>3637</v>
       </c>
       <c r="I1" t="s">
-        <v>2807</v>
+        <v>3638</v>
       </c>
     </row>
     <row r="2">
@@ -10401,7 +12894,7 @@
         <v>2015</v>
       </c>
       <c r="I2" t="s">
-        <v>2808</v>
+        <v>3639</v>
       </c>
     </row>
     <row r="3">
@@ -10428,7 +12921,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>2809</v>
+        <v>3640</v>
       </c>
     </row>
     <row r="4">
@@ -10455,7 +12948,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>2810</v>
+        <v>3641</v>
       </c>
     </row>
     <row r="5">
@@ -10482,7 +12975,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>2811</v>
+        <v>3642</v>
       </c>
     </row>
     <row r="6">
@@ -10509,7 +13002,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>2812</v>
+        <v>3643</v>
       </c>
     </row>
     <row r="7">
@@ -10536,7 +13029,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>2813</v>
+        <v>3644</v>
       </c>
     </row>
     <row r="8">
@@ -10563,7 +13056,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>2814</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="9">
@@ -10590,7 +13083,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>2815</v>
+        <v>3646</v>
       </c>
     </row>
     <row r="10">
@@ -10617,7 +13110,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>2816</v>
+        <v>3647</v>
       </c>
     </row>
     <row r="11">
@@ -10644,7 +13137,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>2817</v>
+        <v>3648</v>
       </c>
     </row>
     <row r="12">
@@ -10671,7 +13164,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>2818</v>
+        <v>3649</v>
       </c>
     </row>
     <row r="13">
@@ -10698,7 +13191,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>2819</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="14">
@@ -10725,7 +13218,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>2820</v>
+        <v>3651</v>
       </c>
     </row>
     <row r="15">
@@ -10752,7 +13245,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>2821</v>
+        <v>3652</v>
       </c>
     </row>
     <row r="16">
@@ -10779,7 +13272,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>2822</v>
+        <v>3653</v>
       </c>
     </row>
     <row r="17">
@@ -10806,7 +13299,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>2823</v>
+        <v>3654</v>
       </c>
     </row>
     <row r="18">
@@ -10833,7 +13326,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>2824</v>
+        <v>3655</v>
       </c>
     </row>
     <row r="19">
@@ -10860,7 +13353,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>2825</v>
+        <v>3656</v>
       </c>
     </row>
     <row r="20">
@@ -10887,7 +13380,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>2826</v>
+        <v>3657</v>
       </c>
     </row>
     <row r="21">
@@ -10914,7 +13407,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" t="s">
-        <v>2827</v>
+        <v>3658</v>
       </c>
     </row>
   </sheetData>
@@ -10928,31 +13421,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>2828</v>
+        <v>3659</v>
       </c>
       <c r="B1" t="s">
-        <v>2829</v>
+        <v>3660</v>
       </c>
       <c r="C1" t="s">
-        <v>2830</v>
+        <v>3661</v>
       </c>
       <c r="D1" t="s">
-        <v>2831</v>
+        <v>3662</v>
       </c>
       <c r="E1" t="s">
-        <v>2832</v>
+        <v>3663</v>
       </c>
       <c r="F1" t="s">
-        <v>2833</v>
+        <v>3664</v>
       </c>
       <c r="G1" t="s">
-        <v>2834</v>
+        <v>3665</v>
       </c>
       <c r="H1" t="s">
-        <v>2835</v>
+        <v>3666</v>
       </c>
       <c r="I1" t="s">
-        <v>2836</v>
+        <v>3667</v>
       </c>
     </row>
     <row r="2">
@@ -10981,7 +13474,7 @@
         <v>2016</v>
       </c>
       <c r="I2" t="s">
-        <v>2837</v>
+        <v>3668</v>
       </c>
     </row>
     <row r="3">
@@ -11008,7 +13501,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>2838</v>
+        <v>3669</v>
       </c>
     </row>
     <row r="4">
@@ -11035,7 +13528,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>2839</v>
+        <v>3670</v>
       </c>
     </row>
     <row r="5">
@@ -11062,7 +13555,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>2840</v>
+        <v>3671</v>
       </c>
     </row>
     <row r="6">
@@ -11089,7 +13582,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>2841</v>
+        <v>3672</v>
       </c>
     </row>
     <row r="7">
@@ -11116,7 +13609,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>2842</v>
+        <v>3673</v>
       </c>
     </row>
     <row r="8">
@@ -11143,7 +13636,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>2843</v>
+        <v>3674</v>
       </c>
     </row>
     <row r="9">
@@ -11170,7 +13663,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>2844</v>
+        <v>3675</v>
       </c>
     </row>
     <row r="10">
@@ -11197,7 +13690,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>2845</v>
+        <v>3676</v>
       </c>
     </row>
     <row r="11">
@@ -11224,7 +13717,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>2846</v>
+        <v>3677</v>
       </c>
     </row>
     <row r="12">
@@ -11251,7 +13744,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>2847</v>
+        <v>3678</v>
       </c>
     </row>
     <row r="13">
@@ -11278,7 +13771,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>2848</v>
+        <v>3679</v>
       </c>
     </row>
     <row r="14">
@@ -11305,7 +13798,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>2849</v>
+        <v>3680</v>
       </c>
     </row>
     <row r="15">
@@ -11332,7 +13825,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>2850</v>
+        <v>3681</v>
       </c>
     </row>
     <row r="16">
@@ -11359,7 +13852,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>2851</v>
+        <v>3682</v>
       </c>
     </row>
     <row r="17">
@@ -11386,7 +13879,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>2852</v>
+        <v>3683</v>
       </c>
     </row>
     <row r="18">
@@ -11413,7 +13906,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>2853</v>
+        <v>3684</v>
       </c>
     </row>
     <row r="19">
@@ -11440,7 +13933,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>2854</v>
+        <v>3685</v>
       </c>
     </row>
     <row r="20">
@@ -11467,7 +13960,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>2855</v>
+        <v>3686</v>
       </c>
     </row>
     <row r="21">
@@ -11494,7 +13987,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" t="s">
-        <v>2856</v>
+        <v>3687</v>
       </c>
     </row>
     <row r="22">
@@ -11521,7 +14014,7 @@
       </c>
       <c r="H22" s="1"/>
       <c r="I22" t="s">
-        <v>2857</v>
+        <v>3688</v>
       </c>
     </row>
   </sheetData>
@@ -11535,31 +14028,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>2858</v>
+        <v>3689</v>
       </c>
       <c r="B1" t="s">
-        <v>2859</v>
+        <v>3690</v>
       </c>
       <c r="C1" t="s">
-        <v>2860</v>
+        <v>3691</v>
       </c>
       <c r="D1" t="s">
-        <v>2861</v>
+        <v>3692</v>
       </c>
       <c r="E1" t="s">
-        <v>2862</v>
+        <v>3693</v>
       </c>
       <c r="F1" t="s">
-        <v>2863</v>
+        <v>3694</v>
       </c>
       <c r="G1" t="s">
-        <v>2864</v>
+        <v>3695</v>
       </c>
       <c r="H1" t="s">
-        <v>2865</v>
+        <v>3696</v>
       </c>
       <c r="I1" t="s">
-        <v>2866</v>
+        <v>3697</v>
       </c>
     </row>
     <row r="2">
@@ -11588,7 +14081,7 @@
         <v>2017</v>
       </c>
       <c r="I2" t="s">
-        <v>2867</v>
+        <v>3698</v>
       </c>
     </row>
     <row r="3">
@@ -11615,7 +14108,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>2868</v>
+        <v>3699</v>
       </c>
     </row>
     <row r="4">
@@ -11642,7 +14135,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>2869</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="5">
@@ -11669,7 +14162,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>2870</v>
+        <v>3701</v>
       </c>
     </row>
     <row r="6">
@@ -11696,7 +14189,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>2871</v>
+        <v>3702</v>
       </c>
     </row>
     <row r="7">
@@ -11723,7 +14216,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>2872</v>
+        <v>3703</v>
       </c>
     </row>
     <row r="8">
@@ -11750,7 +14243,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>2873</v>
+        <v>3704</v>
       </c>
     </row>
     <row r="9">
@@ -11777,7 +14270,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>2874</v>
+        <v>3705</v>
       </c>
     </row>
     <row r="10">
@@ -11804,7 +14297,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>2875</v>
+        <v>3706</v>
       </c>
     </row>
     <row r="11">
@@ -11831,7 +14324,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>2876</v>
+        <v>3707</v>
       </c>
     </row>
     <row r="12">
@@ -11858,7 +14351,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>2877</v>
+        <v>3708</v>
       </c>
     </row>
     <row r="13">
@@ -11885,7 +14378,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>2878</v>
+        <v>3709</v>
       </c>
     </row>
     <row r="14">
@@ -11912,7 +14405,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>2879</v>
+        <v>3710</v>
       </c>
     </row>
     <row r="15">
@@ -11939,7 +14432,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>2880</v>
+        <v>3711</v>
       </c>
     </row>
     <row r="16">
@@ -11966,7 +14459,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>2881</v>
+        <v>3712</v>
       </c>
     </row>
     <row r="17">
@@ -11993,7 +14486,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>2882</v>
+        <v>3713</v>
       </c>
     </row>
     <row r="18">
@@ -12020,7 +14513,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>2883</v>
+        <v>3714</v>
       </c>
     </row>
     <row r="19">
@@ -12047,7 +14540,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>2884</v>
+        <v>3715</v>
       </c>
     </row>
     <row r="20">
@@ -12074,7 +14567,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>2885</v>
+        <v>3716</v>
       </c>
     </row>
   </sheetData>
@@ -12088,31 +14581,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>2886</v>
+        <v>3717</v>
       </c>
       <c r="B1" t="s">
-        <v>2887</v>
+        <v>3718</v>
       </c>
       <c r="C1" t="s">
-        <v>2888</v>
+        <v>3719</v>
       </c>
       <c r="D1" t="s">
-        <v>2889</v>
+        <v>3720</v>
       </c>
       <c r="E1" t="s">
-        <v>2890</v>
+        <v>3721</v>
       </c>
       <c r="F1" t="s">
-        <v>2891</v>
+        <v>3722</v>
       </c>
       <c r="G1" t="s">
-        <v>2892</v>
+        <v>3723</v>
       </c>
       <c r="H1" t="s">
-        <v>2893</v>
+        <v>3724</v>
       </c>
       <c r="I1" t="s">
-        <v>2894</v>
+        <v>3725</v>
       </c>
     </row>
     <row r="2">
@@ -12141,7 +14634,7 @@
         <v>2018</v>
       </c>
       <c r="I2" t="s">
-        <v>2895</v>
+        <v>3726</v>
       </c>
     </row>
     <row r="3">
@@ -12168,7 +14661,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>2896</v>
+        <v>3727</v>
       </c>
     </row>
     <row r="4">
@@ -12195,7 +14688,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>2897</v>
+        <v>3728</v>
       </c>
     </row>
     <row r="5">
@@ -12222,7 +14715,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>2898</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="6">
@@ -12249,7 +14742,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>2899</v>
+        <v>3730</v>
       </c>
     </row>
     <row r="7">
@@ -12276,7 +14769,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>2900</v>
+        <v>3731</v>
       </c>
     </row>
     <row r="8">
@@ -12303,7 +14796,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>2901</v>
+        <v>3732</v>
       </c>
     </row>
     <row r="9">
@@ -12330,7 +14823,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>2902</v>
+        <v>3733</v>
       </c>
     </row>
     <row r="10">
@@ -12357,7 +14850,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>2903</v>
+        <v>3734</v>
       </c>
     </row>
     <row r="11">
@@ -12384,7 +14877,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>2904</v>
+        <v>3735</v>
       </c>
     </row>
     <row r="12">
@@ -12411,7 +14904,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>2905</v>
+        <v>3736</v>
       </c>
     </row>
     <row r="13">
@@ -12438,7 +14931,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>2906</v>
+        <v>3737</v>
       </c>
     </row>
     <row r="14">
@@ -12465,7 +14958,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>2907</v>
+        <v>3738</v>
       </c>
     </row>
     <row r="15">
@@ -12492,7 +14985,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>2908</v>
+        <v>3739</v>
       </c>
     </row>
     <row r="16">
@@ -12519,7 +15012,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>2909</v>
+        <v>3740</v>
       </c>
     </row>
     <row r="17">
@@ -12546,7 +15039,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>2910</v>
+        <v>3741</v>
       </c>
     </row>
     <row r="18">
@@ -12573,7 +15066,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>2911</v>
+        <v>3742</v>
       </c>
     </row>
     <row r="19">
@@ -12600,7 +15093,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>2912</v>
+        <v>3743</v>
       </c>
     </row>
   </sheetData>
@@ -12614,31 +15107,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>2913</v>
+        <v>3744</v>
       </c>
       <c r="B1" t="s">
-        <v>2914</v>
+        <v>3745</v>
       </c>
       <c r="C1" t="s">
-        <v>2915</v>
+        <v>3746</v>
       </c>
       <c r="D1" t="s">
-        <v>2916</v>
+        <v>3747</v>
       </c>
       <c r="E1" t="s">
-        <v>2917</v>
+        <v>3748</v>
       </c>
       <c r="F1" t="s">
-        <v>2918</v>
+        <v>3749</v>
       </c>
       <c r="G1" t="s">
-        <v>2919</v>
+        <v>3750</v>
       </c>
       <c r="H1" t="s">
-        <v>2920</v>
+        <v>3751</v>
       </c>
       <c r="I1" t="s">
-        <v>2921</v>
+        <v>3752</v>
       </c>
     </row>
     <row r="2">
@@ -12667,7 +15160,7 @@
         <v>2019</v>
       </c>
       <c r="I2" t="s">
-        <v>2922</v>
+        <v>3753</v>
       </c>
     </row>
     <row r="3">
@@ -12694,7 +15187,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>2923</v>
+        <v>3754</v>
       </c>
     </row>
     <row r="4">
@@ -12721,7 +15214,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>2924</v>
+        <v>3755</v>
       </c>
     </row>
     <row r="5">
@@ -12748,7 +15241,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>2925</v>
+        <v>3756</v>
       </c>
     </row>
     <row r="6">
@@ -12775,7 +15268,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>2926</v>
+        <v>3757</v>
       </c>
     </row>
     <row r="7">
@@ -12802,7 +15295,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>2927</v>
+        <v>3758</v>
       </c>
     </row>
     <row r="8">
@@ -12829,7 +15322,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>2928</v>
+        <v>3759</v>
       </c>
     </row>
     <row r="9">
@@ -12856,7 +15349,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>2929</v>
+        <v>3760</v>
       </c>
     </row>
     <row r="10">
@@ -12883,7 +15376,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>2930</v>
+        <v>3761</v>
       </c>
     </row>
     <row r="11">
@@ -12910,7 +15403,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>2931</v>
+        <v>3762</v>
       </c>
     </row>
     <row r="12">
@@ -12937,7 +15430,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>2932</v>
+        <v>3763</v>
       </c>
     </row>
     <row r="13">
@@ -12964,7 +15457,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>2933</v>
+        <v>3764</v>
       </c>
     </row>
     <row r="14">
@@ -12991,7 +15484,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>2934</v>
+        <v>3765</v>
       </c>
     </row>
     <row r="15">
@@ -13018,7 +15511,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>2935</v>
+        <v>3766</v>
       </c>
     </row>
     <row r="16">
@@ -13045,7 +15538,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>2936</v>
+        <v>3767</v>
       </c>
     </row>
     <row r="17">
@@ -13072,7 +15565,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>2937</v>
+        <v>3768</v>
       </c>
     </row>
     <row r="18">
@@ -13099,7 +15592,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>2938</v>
+        <v>3769</v>
       </c>
     </row>
     <row r="19">
@@ -13126,7 +15619,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>2939</v>
+        <v>3770</v>
       </c>
     </row>
   </sheetData>
@@ -13140,31 +15633,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>2940</v>
+        <v>3771</v>
       </c>
       <c r="B1" t="s">
-        <v>2941</v>
+        <v>3772</v>
       </c>
       <c r="C1" t="s">
-        <v>2942</v>
+        <v>3773</v>
       </c>
       <c r="D1" t="s">
-        <v>2943</v>
+        <v>3774</v>
       </c>
       <c r="E1" t="s">
-        <v>2944</v>
+        <v>3775</v>
       </c>
       <c r="F1" t="s">
-        <v>2945</v>
+        <v>3776</v>
       </c>
       <c r="G1" t="s">
-        <v>2946</v>
+        <v>3777</v>
       </c>
       <c r="H1" t="s">
-        <v>2947</v>
+        <v>3778</v>
       </c>
       <c r="I1" t="s">
-        <v>2948</v>
+        <v>3779</v>
       </c>
     </row>
     <row r="2">
@@ -13193,7 +15686,7 @@
         <v>2020</v>
       </c>
       <c r="I2" t="s">
-        <v>2949</v>
+        <v>3780</v>
       </c>
     </row>
     <row r="3">
@@ -13220,7 +15713,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>2950</v>
+        <v>3781</v>
       </c>
     </row>
     <row r="4">
@@ -13247,7 +15740,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>2951</v>
+        <v>3782</v>
       </c>
     </row>
     <row r="5">
@@ -13274,7 +15767,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>2952</v>
+        <v>3783</v>
       </c>
     </row>
     <row r="6">
@@ -13301,7 +15794,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>2953</v>
+        <v>3784</v>
       </c>
     </row>
     <row r="7">
@@ -13328,7 +15821,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>2954</v>
+        <v>3785</v>
       </c>
     </row>
     <row r="8">
@@ -13355,7 +15848,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>2955</v>
+        <v>3786</v>
       </c>
     </row>
     <row r="9">
@@ -13382,7 +15875,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>2956</v>
+        <v>3787</v>
       </c>
     </row>
     <row r="10">
@@ -13409,7 +15902,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>2957</v>
+        <v>3788</v>
       </c>
     </row>
     <row r="11">
@@ -13436,7 +15929,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>2958</v>
+        <v>3789</v>
       </c>
     </row>
     <row r="12">
@@ -13463,7 +15956,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>2959</v>
+        <v>3790</v>
       </c>
     </row>
     <row r="13">
@@ -13490,7 +15983,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>2960</v>
+        <v>3791</v>
       </c>
     </row>
     <row r="14">
@@ -13517,7 +16010,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>2961</v>
+        <v>3792</v>
       </c>
     </row>
     <row r="15">
@@ -13544,7 +16037,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>2962</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="16">
@@ -13571,7 +16064,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>2963</v>
+        <v>3794</v>
       </c>
     </row>
     <row r="17">
@@ -13598,7 +16091,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>2964</v>
+        <v>3795</v>
       </c>
     </row>
     <row r="18">
@@ -13625,7 +16118,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>2965</v>
+        <v>3796</v>
       </c>
     </row>
   </sheetData>
@@ -13639,31 +16132,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>2966</v>
+        <v>3797</v>
       </c>
       <c r="B1" t="s">
-        <v>2967</v>
+        <v>3798</v>
       </c>
       <c r="C1" t="s">
-        <v>2968</v>
+        <v>3799</v>
       </c>
       <c r="D1" t="s">
-        <v>2969</v>
+        <v>3800</v>
       </c>
       <c r="E1" t="s">
-        <v>2970</v>
+        <v>3801</v>
       </c>
       <c r="F1" t="s">
-        <v>2971</v>
+        <v>3802</v>
       </c>
       <c r="G1" t="s">
-        <v>2972</v>
+        <v>3803</v>
       </c>
       <c r="H1" t="s">
-        <v>2973</v>
+        <v>3804</v>
       </c>
       <c r="I1" t="s">
-        <v>2974</v>
+        <v>3805</v>
       </c>
     </row>
     <row r="2">
@@ -13692,7 +16185,7 @@
         <v>2021</v>
       </c>
       <c r="I2" t="s">
-        <v>2975</v>
+        <v>3806</v>
       </c>
     </row>
     <row r="3">
@@ -13719,7 +16212,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>2976</v>
+        <v>3807</v>
       </c>
     </row>
     <row r="4">
@@ -13746,7 +16239,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>2977</v>
+        <v>3808</v>
       </c>
     </row>
     <row r="5">
@@ -13773,7 +16266,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>2978</v>
+        <v>3809</v>
       </c>
     </row>
     <row r="6">
@@ -13800,7 +16293,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>2979</v>
+        <v>3810</v>
       </c>
     </row>
     <row r="7">
@@ -13827,7 +16320,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>2980</v>
+        <v>3811</v>
       </c>
     </row>
     <row r="8">
@@ -13854,7 +16347,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>2981</v>
+        <v>3812</v>
       </c>
     </row>
     <row r="9">
@@ -13881,7 +16374,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>2982</v>
+        <v>3813</v>
       </c>
     </row>
     <row r="10">
@@ -13908,7 +16401,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>2983</v>
+        <v>3814</v>
       </c>
     </row>
     <row r="11">
@@ -13935,7 +16428,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>2984</v>
+        <v>3815</v>
       </c>
     </row>
     <row r="12">
@@ -13962,7 +16455,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>2985</v>
+        <v>3816</v>
       </c>
     </row>
     <row r="13">
@@ -13989,7 +16482,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>2986</v>
+        <v>3817</v>
       </c>
     </row>
     <row r="14">
@@ -14016,7 +16509,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>2987</v>
+        <v>3818</v>
       </c>
     </row>
     <row r="15">
@@ -14043,7 +16536,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>2988</v>
+        <v>3819</v>
       </c>
     </row>
     <row r="16">
@@ -14070,7 +16563,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>2989</v>
+        <v>3820</v>
       </c>
     </row>
     <row r="17">
@@ -14097,7 +16590,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>2990</v>
+        <v>3821</v>
       </c>
     </row>
     <row r="18">
@@ -14124,7 +16617,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>2991</v>
+        <v>3822</v>
       </c>
     </row>
   </sheetData>
@@ -14138,31 +16631,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>2992</v>
+        <v>3823</v>
       </c>
       <c r="B1" t="s">
-        <v>2993</v>
+        <v>3824</v>
       </c>
       <c r="C1" t="s">
-        <v>2994</v>
+        <v>3825</v>
       </c>
       <c r="D1" t="s">
-        <v>2995</v>
+        <v>3826</v>
       </c>
       <c r="E1" t="s">
-        <v>2996</v>
+        <v>3827</v>
       </c>
       <c r="F1" t="s">
-        <v>2997</v>
+        <v>3828</v>
       </c>
       <c r="G1" t="s">
-        <v>2998</v>
+        <v>3829</v>
       </c>
       <c r="H1" t="s">
-        <v>2999</v>
+        <v>3830</v>
       </c>
       <c r="I1" t="s">
-        <v>3000</v>
+        <v>3831</v>
       </c>
     </row>
     <row r="2">
@@ -14191,7 +16684,7 @@
         <v>2022</v>
       </c>
       <c r="I2" t="s">
-        <v>3001</v>
+        <v>3832</v>
       </c>
     </row>
     <row r="3">
@@ -14218,7 +16711,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>3002</v>
+        <v>3833</v>
       </c>
     </row>
     <row r="4">
@@ -14245,7 +16738,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>3003</v>
+        <v>3834</v>
       </c>
     </row>
     <row r="5">
@@ -14272,7 +16765,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>3004</v>
+        <v>3835</v>
       </c>
     </row>
     <row r="6">
@@ -14299,7 +16792,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>3005</v>
+        <v>3836</v>
       </c>
     </row>
     <row r="7">
@@ -14326,7 +16819,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>3006</v>
+        <v>3837</v>
       </c>
     </row>
     <row r="8">
@@ -14353,7 +16846,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>3007</v>
+        <v>3838</v>
       </c>
     </row>
     <row r="9">
@@ -14380,7 +16873,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>3008</v>
+        <v>3839</v>
       </c>
     </row>
     <row r="10">
@@ -14407,7 +16900,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>3009</v>
+        <v>3840</v>
       </c>
     </row>
     <row r="11">
@@ -14434,7 +16927,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>3010</v>
+        <v>3841</v>
       </c>
     </row>
     <row r="12">
@@ -14461,7 +16954,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>3011</v>
+        <v>3842</v>
       </c>
     </row>
     <row r="13">
@@ -14488,7 +16981,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>3012</v>
+        <v>3843</v>
       </c>
     </row>
     <row r="14">
@@ -14515,7 +17008,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>3013</v>
+        <v>3844</v>
       </c>
     </row>
     <row r="15">
@@ -14542,7 +17035,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>3014</v>
+        <v>3845</v>
       </c>
     </row>
     <row r="16">
@@ -14569,7 +17062,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>3015</v>
+        <v>3846</v>
       </c>
     </row>
     <row r="17">
@@ -14596,7 +17089,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>3016</v>
+        <v>3847</v>
       </c>
     </row>
     <row r="18">
@@ -14623,7 +17116,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>3017</v>
+        <v>3848</v>
       </c>
     </row>
     <row r="19">
@@ -14650,7 +17143,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>3018</v>
+        <v>3849</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solve monotonicity problems and plot b20
</commit_message>
<xml_diff>
--- a/input_data/admin_data/COL/_clean/total-pos-COL.xlsx
+++ b/input_data/admin_data/COL/_clean/total-pos-COL.xlsx
@@ -22,7 +22,838 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3878" uniqueCount="3878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4155" uniqueCount="4155">
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>poptot</t>
+  </si>
+  <si>
+    <t>thr</t>
+  </si>
+  <si>
+    <t>topavg</t>
+  </si>
+  <si>
+    <t>bracketavg</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>eff_tax_rate</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t/>
+  </si>
   <si>
     <t>poptot</t>
   </si>
@@ -11708,31 +12539,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>3601</v>
+        <v>3878</v>
       </c>
       <c r="B1" t="s">
-        <v>3602</v>
+        <v>3879</v>
       </c>
       <c r="C1" t="s">
-        <v>3603</v>
+        <v>3880</v>
       </c>
       <c r="D1" t="s">
-        <v>3604</v>
+        <v>3881</v>
       </c>
       <c r="E1" t="s">
-        <v>3605</v>
+        <v>3882</v>
       </c>
       <c r="F1" t="s">
-        <v>3606</v>
+        <v>3883</v>
       </c>
       <c r="G1" t="s">
-        <v>3607</v>
+        <v>3884</v>
       </c>
       <c r="H1" t="s">
-        <v>3608</v>
+        <v>3885</v>
       </c>
       <c r="I1" t="s">
-        <v>3609</v>
+        <v>3886</v>
       </c>
     </row>
     <row r="2">
@@ -11761,7 +12592,7 @@
         <v>2014</v>
       </c>
       <c r="I2" t="s">
-        <v>3610</v>
+        <v>3887</v>
       </c>
     </row>
     <row r="3">
@@ -11788,7 +12619,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>3611</v>
+        <v>3888</v>
       </c>
     </row>
     <row r="4">
@@ -11815,7 +12646,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>3612</v>
+        <v>3889</v>
       </c>
     </row>
     <row r="5">
@@ -11842,7 +12673,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>3613</v>
+        <v>3890</v>
       </c>
     </row>
     <row r="6">
@@ -11869,7 +12700,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>3614</v>
+        <v>3891</v>
       </c>
     </row>
     <row r="7">
@@ -11896,7 +12727,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>3615</v>
+        <v>3892</v>
       </c>
     </row>
     <row r="8">
@@ -11923,7 +12754,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>3616</v>
+        <v>3893</v>
       </c>
     </row>
     <row r="9">
@@ -11950,7 +12781,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>3617</v>
+        <v>3894</v>
       </c>
     </row>
     <row r="10">
@@ -11977,7 +12808,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>3618</v>
+        <v>3895</v>
       </c>
     </row>
     <row r="11">
@@ -12004,7 +12835,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>3619</v>
+        <v>3896</v>
       </c>
     </row>
     <row r="12">
@@ -12031,7 +12862,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>3620</v>
+        <v>3897</v>
       </c>
     </row>
     <row r="13">
@@ -12058,7 +12889,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>3621</v>
+        <v>3898</v>
       </c>
     </row>
     <row r="14">
@@ -12085,7 +12916,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>3622</v>
+        <v>3899</v>
       </c>
     </row>
     <row r="15">
@@ -12112,7 +12943,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>3623</v>
+        <v>3900</v>
       </c>
     </row>
     <row r="16">
@@ -12139,7 +12970,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>3624</v>
+        <v>3901</v>
       </c>
     </row>
     <row r="17">
@@ -12166,7 +12997,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>3625</v>
+        <v>3902</v>
       </c>
     </row>
     <row r="18">
@@ -12193,7 +13024,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>3626</v>
+        <v>3903</v>
       </c>
     </row>
     <row r="19">
@@ -12220,7 +13051,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>3627</v>
+        <v>3904</v>
       </c>
     </row>
     <row r="20">
@@ -12247,7 +13078,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>3628</v>
+        <v>3905</v>
       </c>
     </row>
     <row r="21">
@@ -12274,7 +13105,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" t="s">
-        <v>3629</v>
+        <v>3906</v>
       </c>
     </row>
   </sheetData>
@@ -12288,31 +13119,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>3850</v>
+        <v>4127</v>
       </c>
       <c r="B1" t="s">
-        <v>3851</v>
+        <v>4128</v>
       </c>
       <c r="C1" t="s">
-        <v>3852</v>
+        <v>4129</v>
       </c>
       <c r="D1" t="s">
-        <v>3853</v>
+        <v>4130</v>
       </c>
       <c r="E1" t="s">
-        <v>3854</v>
+        <v>4131</v>
       </c>
       <c r="F1" t="s">
-        <v>3855</v>
+        <v>4132</v>
       </c>
       <c r="G1" t="s">
-        <v>3856</v>
+        <v>4133</v>
       </c>
       <c r="H1" t="s">
-        <v>3857</v>
+        <v>4134</v>
       </c>
       <c r="I1" t="s">
-        <v>3858</v>
+        <v>4135</v>
       </c>
     </row>
     <row r="2">
@@ -12341,7 +13172,7 @@
         <v>2023</v>
       </c>
       <c r="I2" t="s">
-        <v>3859</v>
+        <v>4136</v>
       </c>
     </row>
     <row r="3">
@@ -12368,7 +13199,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>3860</v>
+        <v>4137</v>
       </c>
     </row>
     <row r="4">
@@ -12395,7 +13226,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>3861</v>
+        <v>4138</v>
       </c>
     </row>
     <row r="5">
@@ -12422,7 +13253,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>3862</v>
+        <v>4139</v>
       </c>
     </row>
     <row r="6">
@@ -12449,7 +13280,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>3863</v>
+        <v>4140</v>
       </c>
     </row>
     <row r="7">
@@ -12476,7 +13307,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>3864</v>
+        <v>4141</v>
       </c>
     </row>
     <row r="8">
@@ -12503,7 +13334,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>3865</v>
+        <v>4142</v>
       </c>
     </row>
     <row r="9">
@@ -12530,7 +13361,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>3866</v>
+        <v>4143</v>
       </c>
     </row>
     <row r="10">
@@ -12557,7 +13388,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>3867</v>
+        <v>4144</v>
       </c>
     </row>
     <row r="11">
@@ -12584,7 +13415,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>3868</v>
+        <v>4145</v>
       </c>
     </row>
     <row r="12">
@@ -12611,7 +13442,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>3869</v>
+        <v>4146</v>
       </c>
     </row>
     <row r="13">
@@ -12638,7 +13469,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>3870</v>
+        <v>4147</v>
       </c>
     </row>
     <row r="14">
@@ -12665,7 +13496,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>3871</v>
+        <v>4148</v>
       </c>
     </row>
     <row r="15">
@@ -12692,7 +13523,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>3872</v>
+        <v>4149</v>
       </c>
     </row>
     <row r="16">
@@ -12719,7 +13550,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>3873</v>
+        <v>4150</v>
       </c>
     </row>
     <row r="17">
@@ -12746,7 +13577,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>3874</v>
+        <v>4151</v>
       </c>
     </row>
     <row r="18">
@@ -12773,7 +13604,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>3875</v>
+        <v>4152</v>
       </c>
     </row>
     <row r="19">
@@ -12800,7 +13631,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>3876</v>
+        <v>4153</v>
       </c>
     </row>
     <row r="20">
@@ -12827,7 +13658,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>3877</v>
+        <v>4154</v>
       </c>
     </row>
   </sheetData>
@@ -12841,31 +13672,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>3630</v>
+        <v>3907</v>
       </c>
       <c r="B1" t="s">
-        <v>3631</v>
+        <v>3908</v>
       </c>
       <c r="C1" t="s">
-        <v>3632</v>
+        <v>3909</v>
       </c>
       <c r="D1" t="s">
-        <v>3633</v>
+        <v>3910</v>
       </c>
       <c r="E1" t="s">
-        <v>3634</v>
+        <v>3911</v>
       </c>
       <c r="F1" t="s">
-        <v>3635</v>
+        <v>3912</v>
       </c>
       <c r="G1" t="s">
-        <v>3636</v>
+        <v>3913</v>
       </c>
       <c r="H1" t="s">
-        <v>3637</v>
+        <v>3914</v>
       </c>
       <c r="I1" t="s">
-        <v>3638</v>
+        <v>3915</v>
       </c>
     </row>
     <row r="2">
@@ -12894,7 +13725,7 @@
         <v>2015</v>
       </c>
       <c r="I2" t="s">
-        <v>3639</v>
+        <v>3916</v>
       </c>
     </row>
     <row r="3">
@@ -12921,7 +13752,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>3640</v>
+        <v>3917</v>
       </c>
     </row>
     <row r="4">
@@ -12948,7 +13779,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>3641</v>
+        <v>3918</v>
       </c>
     </row>
     <row r="5">
@@ -12975,7 +13806,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>3642</v>
+        <v>3919</v>
       </c>
     </row>
     <row r="6">
@@ -13002,7 +13833,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>3643</v>
+        <v>3920</v>
       </c>
     </row>
     <row r="7">
@@ -13029,7 +13860,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>3644</v>
+        <v>3921</v>
       </c>
     </row>
     <row r="8">
@@ -13056,7 +13887,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>3645</v>
+        <v>3922</v>
       </c>
     </row>
     <row r="9">
@@ -13083,7 +13914,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>3646</v>
+        <v>3923</v>
       </c>
     </row>
     <row r="10">
@@ -13110,7 +13941,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>3647</v>
+        <v>3924</v>
       </c>
     </row>
     <row r="11">
@@ -13137,7 +13968,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>3648</v>
+        <v>3925</v>
       </c>
     </row>
     <row r="12">
@@ -13164,7 +13995,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>3649</v>
+        <v>3926</v>
       </c>
     </row>
     <row r="13">
@@ -13191,7 +14022,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>3650</v>
+        <v>3927</v>
       </c>
     </row>
     <row r="14">
@@ -13218,7 +14049,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>3651</v>
+        <v>3928</v>
       </c>
     </row>
     <row r="15">
@@ -13245,7 +14076,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>3652</v>
+        <v>3929</v>
       </c>
     </row>
     <row r="16">
@@ -13272,7 +14103,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>3653</v>
+        <v>3930</v>
       </c>
     </row>
     <row r="17">
@@ -13299,7 +14130,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>3654</v>
+        <v>3931</v>
       </c>
     </row>
     <row r="18">
@@ -13326,7 +14157,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>3655</v>
+        <v>3932</v>
       </c>
     </row>
     <row r="19">
@@ -13353,7 +14184,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>3656</v>
+        <v>3933</v>
       </c>
     </row>
     <row r="20">
@@ -13380,7 +14211,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>3657</v>
+        <v>3934</v>
       </c>
     </row>
     <row r="21">
@@ -13407,7 +14238,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" t="s">
-        <v>3658</v>
+        <v>3935</v>
       </c>
     </row>
   </sheetData>
@@ -13421,31 +14252,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>3659</v>
+        <v>3936</v>
       </c>
       <c r="B1" t="s">
-        <v>3660</v>
+        <v>3937</v>
       </c>
       <c r="C1" t="s">
-        <v>3661</v>
+        <v>3938</v>
       </c>
       <c r="D1" t="s">
-        <v>3662</v>
+        <v>3939</v>
       </c>
       <c r="E1" t="s">
-        <v>3663</v>
+        <v>3940</v>
       </c>
       <c r="F1" t="s">
-        <v>3664</v>
+        <v>3941</v>
       </c>
       <c r="G1" t="s">
-        <v>3665</v>
+        <v>3942</v>
       </c>
       <c r="H1" t="s">
-        <v>3666</v>
+        <v>3943</v>
       </c>
       <c r="I1" t="s">
-        <v>3667</v>
+        <v>3944</v>
       </c>
     </row>
     <row r="2">
@@ -13474,7 +14305,7 @@
         <v>2016</v>
       </c>
       <c r="I2" t="s">
-        <v>3668</v>
+        <v>3945</v>
       </c>
     </row>
     <row r="3">
@@ -13501,7 +14332,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>3669</v>
+        <v>3946</v>
       </c>
     </row>
     <row r="4">
@@ -13528,7 +14359,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>3670</v>
+        <v>3947</v>
       </c>
     </row>
     <row r="5">
@@ -13555,7 +14386,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>3671</v>
+        <v>3948</v>
       </c>
     </row>
     <row r="6">
@@ -13582,7 +14413,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>3672</v>
+        <v>3949</v>
       </c>
     </row>
     <row r="7">
@@ -13609,7 +14440,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>3673</v>
+        <v>3950</v>
       </c>
     </row>
     <row r="8">
@@ -13636,7 +14467,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>3674</v>
+        <v>3951</v>
       </c>
     </row>
     <row r="9">
@@ -13663,7 +14494,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>3675</v>
+        <v>3952</v>
       </c>
     </row>
     <row r="10">
@@ -13690,7 +14521,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>3676</v>
+        <v>3953</v>
       </c>
     </row>
     <row r="11">
@@ -13717,7 +14548,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>3677</v>
+        <v>3954</v>
       </c>
     </row>
     <row r="12">
@@ -13744,7 +14575,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>3678</v>
+        <v>3955</v>
       </c>
     </row>
     <row r="13">
@@ -13771,7 +14602,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>3679</v>
+        <v>3956</v>
       </c>
     </row>
     <row r="14">
@@ -13798,7 +14629,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>3680</v>
+        <v>3957</v>
       </c>
     </row>
     <row r="15">
@@ -13825,7 +14656,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>3681</v>
+        <v>3958</v>
       </c>
     </row>
     <row r="16">
@@ -13852,7 +14683,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>3682</v>
+        <v>3959</v>
       </c>
     </row>
     <row r="17">
@@ -13879,7 +14710,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>3683</v>
+        <v>3960</v>
       </c>
     </row>
     <row r="18">
@@ -13906,7 +14737,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>3684</v>
+        <v>3961</v>
       </c>
     </row>
     <row r="19">
@@ -13933,7 +14764,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>3685</v>
+        <v>3962</v>
       </c>
     </row>
     <row r="20">
@@ -13960,7 +14791,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>3686</v>
+        <v>3963</v>
       </c>
     </row>
     <row r="21">
@@ -13987,7 +14818,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" t="s">
-        <v>3687</v>
+        <v>3964</v>
       </c>
     </row>
     <row r="22">
@@ -14014,7 +14845,7 @@
       </c>
       <c r="H22" s="1"/>
       <c r="I22" t="s">
-        <v>3688</v>
+        <v>3965</v>
       </c>
     </row>
   </sheetData>
@@ -14028,31 +14859,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>3689</v>
+        <v>3966</v>
       </c>
       <c r="B1" t="s">
-        <v>3690</v>
+        <v>3967</v>
       </c>
       <c r="C1" t="s">
-        <v>3691</v>
+        <v>3968</v>
       </c>
       <c r="D1" t="s">
-        <v>3692</v>
+        <v>3969</v>
       </c>
       <c r="E1" t="s">
-        <v>3693</v>
+        <v>3970</v>
       </c>
       <c r="F1" t="s">
-        <v>3694</v>
+        <v>3971</v>
       </c>
       <c r="G1" t="s">
-        <v>3695</v>
+        <v>3972</v>
       </c>
       <c r="H1" t="s">
-        <v>3696</v>
+        <v>3973</v>
       </c>
       <c r="I1" t="s">
-        <v>3697</v>
+        <v>3974</v>
       </c>
     </row>
     <row r="2">
@@ -14081,7 +14912,7 @@
         <v>2017</v>
       </c>
       <c r="I2" t="s">
-        <v>3698</v>
+        <v>3975</v>
       </c>
     </row>
     <row r="3">
@@ -14108,7 +14939,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>3699</v>
+        <v>3976</v>
       </c>
     </row>
     <row r="4">
@@ -14135,7 +14966,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>3700</v>
+        <v>3977</v>
       </c>
     </row>
     <row r="5">
@@ -14162,7 +14993,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>3701</v>
+        <v>3978</v>
       </c>
     </row>
     <row r="6">
@@ -14189,7 +15020,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>3702</v>
+        <v>3979</v>
       </c>
     </row>
     <row r="7">
@@ -14216,7 +15047,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>3703</v>
+        <v>3980</v>
       </c>
     </row>
     <row r="8">
@@ -14243,7 +15074,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>3704</v>
+        <v>3981</v>
       </c>
     </row>
     <row r="9">
@@ -14270,7 +15101,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>3705</v>
+        <v>3982</v>
       </c>
     </row>
     <row r="10">
@@ -14297,7 +15128,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>3706</v>
+        <v>3983</v>
       </c>
     </row>
     <row r="11">
@@ -14324,7 +15155,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>3707</v>
+        <v>3984</v>
       </c>
     </row>
     <row r="12">
@@ -14351,7 +15182,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>3708</v>
+        <v>3985</v>
       </c>
     </row>
     <row r="13">
@@ -14378,7 +15209,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>3709</v>
+        <v>3986</v>
       </c>
     </row>
     <row r="14">
@@ -14405,7 +15236,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>3710</v>
+        <v>3987</v>
       </c>
     </row>
     <row r="15">
@@ -14432,7 +15263,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>3711</v>
+        <v>3988</v>
       </c>
     </row>
     <row r="16">
@@ -14459,7 +15290,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>3712</v>
+        <v>3989</v>
       </c>
     </row>
     <row r="17">
@@ -14486,7 +15317,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>3713</v>
+        <v>3990</v>
       </c>
     </row>
     <row r="18">
@@ -14513,7 +15344,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>3714</v>
+        <v>3991</v>
       </c>
     </row>
     <row r="19">
@@ -14540,7 +15371,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>3715</v>
+        <v>3992</v>
       </c>
     </row>
     <row r="20">
@@ -14567,7 +15398,7 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" t="s">
-        <v>3716</v>
+        <v>3993</v>
       </c>
     </row>
   </sheetData>
@@ -14581,31 +15412,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>3717</v>
+        <v>3994</v>
       </c>
       <c r="B1" t="s">
-        <v>3718</v>
+        <v>3995</v>
       </c>
       <c r="C1" t="s">
-        <v>3719</v>
+        <v>3996</v>
       </c>
       <c r="D1" t="s">
-        <v>3720</v>
+        <v>3997</v>
       </c>
       <c r="E1" t="s">
-        <v>3721</v>
+        <v>3998</v>
       </c>
       <c r="F1" t="s">
-        <v>3722</v>
+        <v>3999</v>
       </c>
       <c r="G1" t="s">
-        <v>3723</v>
+        <v>4000</v>
       </c>
       <c r="H1" t="s">
-        <v>3724</v>
+        <v>4001</v>
       </c>
       <c r="I1" t="s">
-        <v>3725</v>
+        <v>4002</v>
       </c>
     </row>
     <row r="2">
@@ -14634,7 +15465,7 @@
         <v>2018</v>
       </c>
       <c r="I2" t="s">
-        <v>3726</v>
+        <v>4003</v>
       </c>
     </row>
     <row r="3">
@@ -14661,7 +15492,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>3727</v>
+        <v>4004</v>
       </c>
     </row>
     <row r="4">
@@ -14688,7 +15519,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>3728</v>
+        <v>4005</v>
       </c>
     </row>
     <row r="5">
@@ -14715,7 +15546,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>3729</v>
+        <v>4006</v>
       </c>
     </row>
     <row r="6">
@@ -14742,7 +15573,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>3730</v>
+        <v>4007</v>
       </c>
     </row>
     <row r="7">
@@ -14769,7 +15600,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>3731</v>
+        <v>4008</v>
       </c>
     </row>
     <row r="8">
@@ -14796,7 +15627,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>3732</v>
+        <v>4009</v>
       </c>
     </row>
     <row r="9">
@@ -14823,7 +15654,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>3733</v>
+        <v>4010</v>
       </c>
     </row>
     <row r="10">
@@ -14850,7 +15681,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>3734</v>
+        <v>4011</v>
       </c>
     </row>
     <row r="11">
@@ -14877,7 +15708,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>3735</v>
+        <v>4012</v>
       </c>
     </row>
     <row r="12">
@@ -14904,7 +15735,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>3736</v>
+        <v>4013</v>
       </c>
     </row>
     <row r="13">
@@ -14931,7 +15762,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>3737</v>
+        <v>4014</v>
       </c>
     </row>
     <row r="14">
@@ -14958,7 +15789,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>3738</v>
+        <v>4015</v>
       </c>
     </row>
     <row r="15">
@@ -14985,7 +15816,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>3739</v>
+        <v>4016</v>
       </c>
     </row>
     <row r="16">
@@ -15012,7 +15843,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>3740</v>
+        <v>4017</v>
       </c>
     </row>
     <row r="17">
@@ -15039,7 +15870,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>3741</v>
+        <v>4018</v>
       </c>
     </row>
     <row r="18">
@@ -15066,7 +15897,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>3742</v>
+        <v>4019</v>
       </c>
     </row>
     <row r="19">
@@ -15093,7 +15924,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>3743</v>
+        <v>4020</v>
       </c>
     </row>
   </sheetData>
@@ -15107,31 +15938,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>3744</v>
+        <v>4021</v>
       </c>
       <c r="B1" t="s">
-        <v>3745</v>
+        <v>4022</v>
       </c>
       <c r="C1" t="s">
-        <v>3746</v>
+        <v>4023</v>
       </c>
       <c r="D1" t="s">
-        <v>3747</v>
+        <v>4024</v>
       </c>
       <c r="E1" t="s">
-        <v>3748</v>
+        <v>4025</v>
       </c>
       <c r="F1" t="s">
-        <v>3749</v>
+        <v>4026</v>
       </c>
       <c r="G1" t="s">
-        <v>3750</v>
+        <v>4027</v>
       </c>
       <c r="H1" t="s">
-        <v>3751</v>
+        <v>4028</v>
       </c>
       <c r="I1" t="s">
-        <v>3752</v>
+        <v>4029</v>
       </c>
     </row>
     <row r="2">
@@ -15160,7 +15991,7 @@
         <v>2019</v>
       </c>
       <c r="I2" t="s">
-        <v>3753</v>
+        <v>4030</v>
       </c>
     </row>
     <row r="3">
@@ -15187,7 +16018,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>3754</v>
+        <v>4031</v>
       </c>
     </row>
     <row r="4">
@@ -15214,7 +16045,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>3755</v>
+        <v>4032</v>
       </c>
     </row>
     <row r="5">
@@ -15241,7 +16072,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>3756</v>
+        <v>4033</v>
       </c>
     </row>
     <row r="6">
@@ -15268,7 +16099,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>3757</v>
+        <v>4034</v>
       </c>
     </row>
     <row r="7">
@@ -15295,7 +16126,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>3758</v>
+        <v>4035</v>
       </c>
     </row>
     <row r="8">
@@ -15322,7 +16153,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>3759</v>
+        <v>4036</v>
       </c>
     </row>
     <row r="9">
@@ -15349,7 +16180,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>3760</v>
+        <v>4037</v>
       </c>
     </row>
     <row r="10">
@@ -15376,7 +16207,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>3761</v>
+        <v>4038</v>
       </c>
     </row>
     <row r="11">
@@ -15403,7 +16234,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>3762</v>
+        <v>4039</v>
       </c>
     </row>
     <row r="12">
@@ -15430,7 +16261,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>3763</v>
+        <v>4040</v>
       </c>
     </row>
     <row r="13">
@@ -15457,7 +16288,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>3764</v>
+        <v>4041</v>
       </c>
     </row>
     <row r="14">
@@ -15484,7 +16315,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>3765</v>
+        <v>4042</v>
       </c>
     </row>
     <row r="15">
@@ -15511,7 +16342,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>3766</v>
+        <v>4043</v>
       </c>
     </row>
     <row r="16">
@@ -15538,7 +16369,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>3767</v>
+        <v>4044</v>
       </c>
     </row>
     <row r="17">
@@ -15565,7 +16396,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>3768</v>
+        <v>4045</v>
       </c>
     </row>
     <row r="18">
@@ -15592,7 +16423,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>3769</v>
+        <v>4046</v>
       </c>
     </row>
     <row r="19">
@@ -15619,7 +16450,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>3770</v>
+        <v>4047</v>
       </c>
     </row>
   </sheetData>
@@ -15633,31 +16464,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>3771</v>
+        <v>4048</v>
       </c>
       <c r="B1" t="s">
-        <v>3772</v>
+        <v>4049</v>
       </c>
       <c r="C1" t="s">
-        <v>3773</v>
+        <v>4050</v>
       </c>
       <c r="D1" t="s">
-        <v>3774</v>
+        <v>4051</v>
       </c>
       <c r="E1" t="s">
-        <v>3775</v>
+        <v>4052</v>
       </c>
       <c r="F1" t="s">
-        <v>3776</v>
+        <v>4053</v>
       </c>
       <c r="G1" t="s">
-        <v>3777</v>
+        <v>4054</v>
       </c>
       <c r="H1" t="s">
-        <v>3778</v>
+        <v>4055</v>
       </c>
       <c r="I1" t="s">
-        <v>3779</v>
+        <v>4056</v>
       </c>
     </row>
     <row r="2">
@@ -15686,7 +16517,7 @@
         <v>2020</v>
       </c>
       <c r="I2" t="s">
-        <v>3780</v>
+        <v>4057</v>
       </c>
     </row>
     <row r="3">
@@ -15713,7 +16544,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>3781</v>
+        <v>4058</v>
       </c>
     </row>
     <row r="4">
@@ -15740,7 +16571,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>3782</v>
+        <v>4059</v>
       </c>
     </row>
     <row r="5">
@@ -15767,7 +16598,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>3783</v>
+        <v>4060</v>
       </c>
     </row>
     <row r="6">
@@ -15794,7 +16625,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>3784</v>
+        <v>4061</v>
       </c>
     </row>
     <row r="7">
@@ -15821,7 +16652,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>3785</v>
+        <v>4062</v>
       </c>
     </row>
     <row r="8">
@@ -15848,7 +16679,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>3786</v>
+        <v>4063</v>
       </c>
     </row>
     <row r="9">
@@ -15875,7 +16706,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>3787</v>
+        <v>4064</v>
       </c>
     </row>
     <row r="10">
@@ -15902,7 +16733,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>3788</v>
+        <v>4065</v>
       </c>
     </row>
     <row r="11">
@@ -15929,7 +16760,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>3789</v>
+        <v>4066</v>
       </c>
     </row>
     <row r="12">
@@ -15956,7 +16787,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>3790</v>
+        <v>4067</v>
       </c>
     </row>
     <row r="13">
@@ -15983,7 +16814,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>3791</v>
+        <v>4068</v>
       </c>
     </row>
     <row r="14">
@@ -16010,7 +16841,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>3792</v>
+        <v>4069</v>
       </c>
     </row>
     <row r="15">
@@ -16037,7 +16868,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>3793</v>
+        <v>4070</v>
       </c>
     </row>
     <row r="16">
@@ -16064,7 +16895,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>3794</v>
+        <v>4071</v>
       </c>
     </row>
     <row r="17">
@@ -16091,7 +16922,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>3795</v>
+        <v>4072</v>
       </c>
     </row>
     <row r="18">
@@ -16118,7 +16949,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>3796</v>
+        <v>4073</v>
       </c>
     </row>
   </sheetData>
@@ -16132,31 +16963,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>3797</v>
+        <v>4074</v>
       </c>
       <c r="B1" t="s">
-        <v>3798</v>
+        <v>4075</v>
       </c>
       <c r="C1" t="s">
-        <v>3799</v>
+        <v>4076</v>
       </c>
       <c r="D1" t="s">
-        <v>3800</v>
+        <v>4077</v>
       </c>
       <c r="E1" t="s">
-        <v>3801</v>
+        <v>4078</v>
       </c>
       <c r="F1" t="s">
-        <v>3802</v>
+        <v>4079</v>
       </c>
       <c r="G1" t="s">
-        <v>3803</v>
+        <v>4080</v>
       </c>
       <c r="H1" t="s">
-        <v>3804</v>
+        <v>4081</v>
       </c>
       <c r="I1" t="s">
-        <v>3805</v>
+        <v>4082</v>
       </c>
     </row>
     <row r="2">
@@ -16185,7 +17016,7 @@
         <v>2021</v>
       </c>
       <c r="I2" t="s">
-        <v>3806</v>
+        <v>4083</v>
       </c>
     </row>
     <row r="3">
@@ -16212,7 +17043,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>3807</v>
+        <v>4084</v>
       </c>
     </row>
     <row r="4">
@@ -16239,7 +17070,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>3808</v>
+        <v>4085</v>
       </c>
     </row>
     <row r="5">
@@ -16266,7 +17097,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>3809</v>
+        <v>4086</v>
       </c>
     </row>
     <row r="6">
@@ -16293,7 +17124,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>3810</v>
+        <v>4087</v>
       </c>
     </row>
     <row r="7">
@@ -16320,7 +17151,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>3811</v>
+        <v>4088</v>
       </c>
     </row>
     <row r="8">
@@ -16347,7 +17178,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>3812</v>
+        <v>4089</v>
       </c>
     </row>
     <row r="9">
@@ -16374,7 +17205,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>3813</v>
+        <v>4090</v>
       </c>
     </row>
     <row r="10">
@@ -16401,7 +17232,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>3814</v>
+        <v>4091</v>
       </c>
     </row>
     <row r="11">
@@ -16428,7 +17259,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>3815</v>
+        <v>4092</v>
       </c>
     </row>
     <row r="12">
@@ -16455,7 +17286,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>3816</v>
+        <v>4093</v>
       </c>
     </row>
     <row r="13">
@@ -16482,7 +17313,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>3817</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="14">
@@ -16509,7 +17340,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>3818</v>
+        <v>4095</v>
       </c>
     </row>
     <row r="15">
@@ -16536,7 +17367,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>3819</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="16">
@@ -16563,7 +17394,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>3820</v>
+        <v>4097</v>
       </c>
     </row>
     <row r="17">
@@ -16590,7 +17421,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>3821</v>
+        <v>4098</v>
       </c>
     </row>
     <row r="18">
@@ -16617,7 +17448,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>3822</v>
+        <v>4099</v>
       </c>
     </row>
   </sheetData>
@@ -16631,31 +17462,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>3823</v>
+        <v>4100</v>
       </c>
       <c r="B1" t="s">
-        <v>3824</v>
+        <v>4101</v>
       </c>
       <c r="C1" t="s">
-        <v>3825</v>
+        <v>4102</v>
       </c>
       <c r="D1" t="s">
-        <v>3826</v>
+        <v>4103</v>
       </c>
       <c r="E1" t="s">
-        <v>3827</v>
+        <v>4104</v>
       </c>
       <c r="F1" t="s">
-        <v>3828</v>
+        <v>4105</v>
       </c>
       <c r="G1" t="s">
-        <v>3829</v>
+        <v>4106</v>
       </c>
       <c r="H1" t="s">
-        <v>3830</v>
+        <v>4107</v>
       </c>
       <c r="I1" t="s">
-        <v>3831</v>
+        <v>4108</v>
       </c>
     </row>
     <row r="2">
@@ -16684,7 +17515,7 @@
         <v>2022</v>
       </c>
       <c r="I2" t="s">
-        <v>3832</v>
+        <v>4109</v>
       </c>
     </row>
     <row r="3">
@@ -16711,7 +17542,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>3833</v>
+        <v>4110</v>
       </c>
     </row>
     <row r="4">
@@ -16738,7 +17569,7 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>3834</v>
+        <v>4111</v>
       </c>
     </row>
     <row r="5">
@@ -16765,7 +17596,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
-        <v>3835</v>
+        <v>4112</v>
       </c>
     </row>
     <row r="6">
@@ -16792,7 +17623,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>3836</v>
+        <v>4113</v>
       </c>
     </row>
     <row r="7">
@@ -16819,7 +17650,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>3837</v>
+        <v>4114</v>
       </c>
     </row>
     <row r="8">
@@ -16846,7 +17677,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>3838</v>
+        <v>4115</v>
       </c>
     </row>
     <row r="9">
@@ -16873,7 +17704,7 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>3839</v>
+        <v>4116</v>
       </c>
     </row>
     <row r="10">
@@ -16900,7 +17731,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>3840</v>
+        <v>4117</v>
       </c>
     </row>
     <row r="11">
@@ -16927,7 +17758,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>3841</v>
+        <v>4118</v>
       </c>
     </row>
     <row r="12">
@@ -16954,7 +17785,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>3842</v>
+        <v>4119</v>
       </c>
     </row>
     <row r="13">
@@ -16981,7 +17812,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>3843</v>
+        <v>4120</v>
       </c>
     </row>
     <row r="14">
@@ -17008,7 +17839,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>3844</v>
+        <v>4121</v>
       </c>
     </row>
     <row r="15">
@@ -17035,7 +17866,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>3845</v>
+        <v>4122</v>
       </c>
     </row>
     <row r="16">
@@ -17062,7 +17893,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>3846</v>
+        <v>4123</v>
       </c>
     </row>
     <row r="17">
@@ -17089,7 +17920,7 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>3847</v>
+        <v>4124</v>
       </c>
     </row>
     <row r="18">
@@ -17116,7 +17947,7 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" t="s">
-        <v>3848</v>
+        <v>4125</v>
       </c>
     </row>
     <row r="19">
@@ -17143,7 +17974,7 @@
       </c>
       <c r="H19" s="1"/>
       <c r="I19" t="s">
-        <v>3849</v>
+        <v>4126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>